<commit_message>
Fixed depth in Excel file
</commit_message>
<xml_diff>
--- a/tools/excel/finma/finma-2023-01.xlsx
+++ b/tools/excel/finma/finma-2023-01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\finma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C11577-6D3F-40A9-A372-20DB9825E19E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAEDF2B-B5D1-441A-BE66-0BD9AFB191B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1332" windowWidth="19812" windowHeight="11628" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1485" yWindow="-15870" windowWidth="25440" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -1448,8 +1448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A123" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E139" sqref="E139"/>
+    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1834,6 +1834,9 @@
       <c r="A31" t="s">
         <v>80</v>
       </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
       <c r="C31" t="s">
         <v>86</v>
       </c>

</xml_diff>

<commit_message>
Fixed ref_id in Excel file
</commit_message>
<xml_diff>
--- a/tools/excel/finma/finma-2023-01.xlsx
+++ b/tools/excel/finma/finma-2023-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\finma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CAEDF2B-B5D1-441A-BE66-0BD9AFB191B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34674602-B821-4E76-B0FB-AFE78883EC33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1485" yWindow="-15870" windowWidth="25440" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="405" uniqueCount="300">
   <si>
     <t>type</t>
   </si>
@@ -1448,8 +1448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2247,9 +2247,6 @@
       <c r="B58">
         <v>3</v>
       </c>
-      <c r="C58" t="s">
-        <v>144</v>
-      </c>
       <c r="D58" t="s">
         <v>145</v>
       </c>

</xml_diff>

<commit_message>
Add English Version in Excel file + YAML
The YAML file contains both English and French versions.
</commit_message>
<xml_diff>
--- a/tools/excel/finma/finma-2023-01.xlsx
+++ b/tools/excel/finma/finma-2023-01.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\finma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FBA48A8-DC88-4221-ADE6-9D1FAC4CFDFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBC348B-A444-42DF-836B-BD9EA0B01118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="-15870" windowWidth="25440" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
     <sheet name="finma_meta" sheetId="2" r:id="rId2"/>
     <sheet name="finma_content" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="574">
   <si>
     <t>type</t>
   </si>
@@ -94,9 +94,6 @@
     <t>publication_date</t>
   </si>
   <si>
-    <t>2025-06-06</t>
-  </si>
-  <si>
     <t>framework</t>
   </si>
   <si>
@@ -936,16 +933,861 @@
   </si>
   <si>
     <t>Les exigences de fonds propres pour les risques opérationnels au sens des art. 89 ss OFR s’appuient sur les Cm 3 à 116 de la circulaire FINMA 2008/21 « Risques opérationnels – banques » jusqu’à l’entrée en vigueur de l’OFR révisée dans le cadre du paquet de révisions des normes finales de Bâle III et de l’ordonnance d’exécution FINMA correspondante.</t>
+  </si>
+  <si>
+    <t>name[en]</t>
+  </si>
+  <si>
+    <t>description[en]</t>
+  </si>
+  <si>
+    <t>annotation[en]</t>
+  </si>
+  <si>
+    <t>I. Subject and scope of application</t>
+  </si>
+  <si>
+    <t>This Circular relates to the rules on the segregation of duties, risk management and internal controls contained in the Banking Ordinance (Arts. 12 and 14e BO, SR 952.02) and the Financial Institutions Ordinance (Arts. 12 and 68 FinIO; SR 954.11) and sets out the corresponding supervisory practice. It takes account of the Basel Committee’s principles for the sound management of operational risk1 and operational resilience2.</t>
+  </si>
+  <si>
+    <t>[1] BCBS Revisions to the Principles for the Sound Management of Operational Risk (31 March 2021).
+[2] BCBS Principles for Operational Resilience (31 March 2021).</t>
+  </si>
+  <si>
+    <t>This Circular applies to banks under Article 1a and persons under Article 1b of the Banking Act (BA; SR 952.0), securities dealers under Article 2 para. 1 let. e and Article 41 of the Financial Institutions Act (FinIA; SR 954.1), and financial groups and financial conglomerates under Article 3c BA and Article 49 FinIA. In the following, banks, persons under Article 1b BA, securities firms, financial groups and financial conglomerates are referred to collectively as “institutions”.</t>
+  </si>
+  <si>
+    <t>II. Definition of terms</t>
+  </si>
+  <si>
+    <t>Operational risk is defined in Article 89 CAO. It refers to the risk of financial loss resulting from inadequate or failed internal processes or systems, inappropriate actions taken by people or mistakes made by them, or from external events. This includes the financial losses that can result from legal or compliance risks. Operational risk management typically also takes other types of damage into account3, provided that these can ultimately also result in financial loss. It does not include strategic risk.</t>
+  </si>
+  <si>
+    <t>[3] For example, negative impact on reputation, possible loss of confidence and loss of clients, negative impact on the market, negative regulatory impact (e.g. possible loss of licence).</t>
+  </si>
+  <si>
+    <t>Inherent risks are operational risks that the institution is exposed to through its products, activities, processes and systems, without taking control or mitigation measures into account.</t>
+  </si>
+  <si>
+    <t>Residual risks are operational risks that the institution is exposed to after taking control and mitigation measures into account.</t>
+  </si>
+  <si>
+    <t>Information and communication technology (ICT) refers to the physical and logical (electronic) architecture of IT and communication systems, the individual hardware and software assets, networks, data and operating environments.</t>
+  </si>
+  <si>
+    <t>Critical data are data that, in view of the institution’s size, complexity, structure, risk profile and business model, are of such crucial significance that they require increased security measures. These are data that are crucial for the successful and sustainable provision of the institution’s services or for regulatory purposes. When assessing and determining the criticality of data, the confidentiality as well as the integrity and availability must be taken into account. Each of these three aspects can determine whether data is classified as critical.</t>
+  </si>
+  <si>
+    <t>Critical processes are processes whose significant disruption endanger the provision of critical functions. They are part of the critical functions.</t>
+  </si>
+  <si>
+    <t>Business continuity management (BCM) refers to the institution-wide approach for recovering the operation of critical processes in the event of a significant disruption going beyond incident management. It defines the response to significant disruptions. Effective BCM reduces the residual risks in connection with significant disruptions.</t>
+  </si>
+  <si>
+    <t>The recovery time objective (RTO) is the time within which an application, system and/or process must be recovered. The recovery point objective (RPO) is the maximum tolerable period during which data is lost.</t>
+  </si>
+  <si>
+    <t>The business continuity plan (BCP) is a forward-looking plan that sets out the necessary procedures, recovery options and alternative resources (the recovery processes) for ensuring continuity and recovering critical processes.</t>
+  </si>
+  <si>
+    <t>The disaster recovery plan (DRP) defines the recovery processes for achieving the recovery goals in the event of a catastrophic failure or destruction of the ICT and taking into account the possible loss of key personnel.</t>
+  </si>
+  <si>
+    <t>Crisis situations are exceptional situations that potentially threaten the institution’s existence, and that cannot be managed with ordinary measures and decision-making authority. They differ from incidents and significant disruptions that can be overcome with incident management in normal operation or with the defined BCPs and DRPs.</t>
+  </si>
+  <si>
+    <t>Critical functions include:</t>
+  </si>
+  <si>
+    <t>a. the activities, processes and services – including the underlying resources necessary for their provision – whose disruption would jeopardise the institution’s continuation or its role on the financial market and thus the proper functioning of the financial markets; and</t>
+  </si>
+  <si>
+    <t>b. the systemically important functions under Article 8 BA.</t>
+  </si>
+  <si>
+    <t>The tolerance for disruption is the extent (e.g. the duration or expected damage) of the disruption of a critical function that the institution is willing to accept, taking severe but plausible scenarios into account. A tolerance for disruption must be defined for each critical function.</t>
+  </si>
+  <si>
+    <t>Operational resilience refers to the institution’s ability to restore its critical functions in case of a disruption within the tolerance for disruption. That is to say, the institution’s ability to identify threats and possible failures, to protect itself from them and to respond to them, to restore normal business operations in the event of disruptions and to learn from them, so as to minimise the impact of disruptions on the provision of critical functions. An operationally resilient institution has designed its operating model in such a way4 that it is less exposed to the risk of disruptions in relation to its critical functions. Operational resilience thus reduces not only the residual risks of disruptions, but also the inherent risk of disruptions occurring. Effective operational risk management helps strengthen the institution’s operational resilience.</t>
+  </si>
+  <si>
+    <t>[4] Often also called resilience by design.</t>
+  </si>
+  <si>
+    <t>III. Principle of proportionality</t>
+  </si>
+  <si>
+    <t>This Circular applies to all addressees. However, the requirements are to be implemented on a case-by-case basis, depending on the size, complexity, structure and risk profile of each institution. FINMA can relax or tighten the rules in individual cases.</t>
+  </si>
+  <si>
+    <t>Banks and securities firms in FINMA Categories 4 and 5 are exempt from complying with margin nos. 33–38, 41–46, 48, 51, 57, 73, 74, 76–78, 80, 87, 92, 93, 96, 103, 104 and 110–112.</t>
+  </si>
+  <si>
+    <t>Institutions under Articles 47a–47e CAO, persons under Article 1b BA, and investment firms (non-proprietarian trading) are also exempt from complying with margin nos. 72, 75, 79 and 105–109.</t>
+  </si>
+  <si>
+    <t>IV. Operational risk management</t>
+  </si>
+  <si>
+    <t>A. Overarching operational risk management</t>
+  </si>
+  <si>
+    <t>Operational risk management forms part of institution-wide risk management under FINMA Circular 2017/1 “Corporate governance – banks”.</t>
+  </si>
+  <si>
+    <t>The board of directors approves the basic principles for the management of operational risks relevant for the institution and monitors their application. Among others, these include the ICT risks, the cyber risks, the risks relating to critical data, the risks resulting from the design and implementation of BCM and, where applicable, the risks from crossborder service business. At least once a year, the board of directors approves the risk tolerance for operational risk in accordance with the risk policy, taking the institution’s strategic and financial goals into account. In doing so it considers the results from the risk and control assessments under margin no. 30. It accepts either the extent to which the institution is exposed to operational risk, or decides to adjust the risk tolerance and make the strategic changes necessary for this5.</t>
+  </si>
+  <si>
+    <t>[5] For example, a change to the business model.</t>
+  </si>
+  <si>
+    <t>The board of directors regularly approves strategies for dealing with ICT, cyber risks, critical data and BCM, and monitors their application.</t>
+  </si>
+  <si>
+    <t>The executive board ensures in a comprehensible way that the operational risks are identified, assessed, limited and monitored, and that the effectiveness of both the design and also of the implementation of this operational risk management is regularly reviewed. It takes risk-specific supplementary or intensified measures in order to limit the inherent risks deemed to be material6 as the situation demands.</t>
+  </si>
+  <si>
+    <t>[6] Often called top risks or key risks.</t>
+  </si>
+  <si>
+    <t>To raise awareness among employees for reducing relevant operational risks, particularly ICT risks, cyber risks, risks with regard to critical data and the risks resulting from the design and implementation of BCM, measures are to be implemented and carried out taking into account their tasks, competencies and responsibilities7.</t>
+  </si>
+  <si>
+    <t>[7] Among other things, this includes carefully selecting employees, ensuring that they are suitably qualified for their tasks, competencies and responsibilities and providing them with continuing education within the context of their activities.</t>
+  </si>
+  <si>
+    <t>If necessary, FINMA will define more stringent requirements for operational risk management for specific topics as part of ongoing supervision. This will be done cautiously and in accordance with the proportionality principle.</t>
+  </si>
+  <si>
+    <t>The operational risks must be categorised in a uniform manner across the institution and listed in an inventory. The categorisation may be performed based on the categorisation of event types used to calculate the minimum capital requirements for operational risk or based on an internal taxonomy. The categorisation must be applied consistently in all areas of the institution and in all components of operational risk management.</t>
+  </si>
+  <si>
+    <t>Internal8 and external9 factors shall be taken into account for identifying operational risks. The identified operational risks shall be assessed in a comprehensible way both from the perspective of inherent as well as residual risks.</t>
+  </si>
+  <si>
+    <t>[8] Internal factors include, for example, changes to products, activities, processes and systems, review results and internal losses resulting from operational risks.
+[9] External factors include, for example, loss events at other institutions, changes in the security situation (e.g. as a result of environmental influences, cyber attacks or terrorism) or changes to the regulatory requirements.</t>
+  </si>
+  <si>
+    <t>The identification and assessment of operational risks shall be based on at least review results10 and regularly conducted risk and control assessments. The risk and control assessments shall take into account the inherent risks, the effectiveness of the existing control and mitigation measures and the residual risks.</t>
+  </si>
+  <si>
+    <t>[10] Review results encompass here results of internal and external audits, where available, as well as results of reviews performed, for example, by the business and organisational areas, the risk control and compliance functions or supervisory authorities.</t>
+  </si>
+  <si>
+    <t>To assess the existing control and mitigation measures, in particular a regular assessment of the effectiveness of key controls must be performed and documented by an independent control body (design effectiveness and operating effectiveness testing). Key controls are those control and mitigation measures that minimise the inherent risks deemed to be material. The separation of tasks, competencies and responsibilities to ensure independence and prevent conflicts of interests shall also be regularly assessed.</t>
+  </si>
+  <si>
+    <t>Ad hoc risk and control assessments shall be conducted prior to major changes in products, activities, processes and systems. These shall take into account the operational risks associated with the change process and the operational risks of the target state. If necessary, the risk tolerance should be adjusted and control and mitigation measures implemented.</t>
+  </si>
+  <si>
+    <t>Depending on the type, scope, complexity and risk of institution-specific products, activities, processes and systems, the following tools and methods shall be applied:</t>
+  </si>
+  <si>
+    <t>a. Systematic collection and analysis of internal loss data and relevant external events associated with operational risk;</t>
+  </si>
+  <si>
+    <t>b. Risk and control indicators for monitoring operational risk and identifying relevant risk increases in a timely manner;</t>
+  </si>
+  <si>
+    <t>c. Scenario analyses and/or estimates of the loss potential in view of or in comparison with the minimum capital requirements for operational risk;</t>
+  </si>
+  <si>
+    <t>d. Comparative analyses (read-across), for example, analyses of the relevance of review results for other areas of the institution or comparisons between the results of the risk and control assessments for various areas.</t>
+  </si>
+  <si>
+    <t>The risk tolerance for operational risk takes account of both the tolerance in relation to inherent11 as well as residual operational risk and is monitored using risk or control indicators.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[11] The risk tolerance in relation to inherent risk takes account of strategic decisions in relation to the business or operating model, for example, tolerance for the inherent risks associated with serving certain client segments or countries, with offering certain products, with using primarily manual processes, with relying on a complex IT infrastructure or with outsourcing certain operations.
+</t>
+  </si>
+  <si>
+    <t>The risk control function reports to the board of directors at least annually and to the executive board at least every six months in accordance with margin nos. 75–76 of FINMA Circ. 17/1 on the operational risks at the top level12 of the categorisation defined in accordance with margin no. 28, on their comparison with the defined risk tolerance, and on details of material internal losses.</t>
+  </si>
+  <si>
+    <t>[12] The top level of the categorisation is often referred to as level 1. The reporting can also take place on a more detailed level.</t>
+  </si>
+  <si>
+    <t>In relation to the relevant ICT and cyber risks, the report for the executive board produced at least annually shall also contain information on the development of these risks, on the effectiveness of the corresponding key controls, and on material internal and external events in connection with these risks.</t>
+  </si>
+  <si>
+    <t>The internal reporting in accordance with margin no. 39 shall contain in addition the following information:</t>
+  </si>
+  <si>
+    <t>• relevant, external factors in accordance with footnote 9,</t>
+  </si>
+  <si>
+    <t>• summary overview of the effectiveness of the key controls in accordance with margin no. 31,</t>
+  </si>
+  <si>
+    <t>• emerging operational risks;</t>
+  </si>
+  <si>
+    <t>• results from the application of additional tools and methods in accordance with margin no. 33.</t>
+  </si>
+  <si>
+    <t>In accordance with the principle of proportionality, for systemically important banks, regular reporting on operational risks shall also be conducted at the level of the business or organisational areas that are exposed to relevant or material operational risks.</t>
+  </si>
+  <si>
+    <t>B. ICT risk management</t>
+  </si>
+  <si>
+    <t>a) ICT strategy and governance</t>
+  </si>
+  <si>
+    <t>The basic expectations for the strategy, governance and raising of awareness in relation to ICT are set out in margin nos. 23–26 and 40.</t>
+  </si>
+  <si>
+    <t>ICT risk management shall take into account relevant internationally recognised standards and practices as well as the influence of new technological developments on the ICT risks.</t>
+  </si>
+  <si>
+    <t>The executive board shall ensure that procedures, processes and controls as well as tasks, competencies and responsibilities are implemented and documented both for change management and for ICT operations (run, maintenance). These shall be adequately resourced with qualified staff.</t>
+  </si>
+  <si>
+    <t>b) Change management</t>
+  </si>
+  <si>
+    <t>Change management shall define the procedures, processes and controls for all phases in the development or procurement of ICT. In each of these phases it shall consider the impact of the change on the ICT risks. It shall focus in particular on the requirements with regard to confidentiality, integrity and availability.</t>
+  </si>
+  <si>
+    <t>It must be ensured that the development or test environments are separate from the ICT production environment. This also involves the clear allocation of tasks, competencies and responsibilities and laying down rules for the associated access rights.</t>
+  </si>
+  <si>
+    <t>When developing and procuring ICT, functional and non-functional requirements13 shall be clearly defined and approved; they shall be tested and validated based on their criticality.</t>
+  </si>
+  <si>
+    <t>[13] E.g. with regard to architecture or information security requirements.</t>
+  </si>
+  <si>
+    <t>c) ICT operations (run, maintenance)</t>
+  </si>
+  <si>
+    <t>The institution shall keep one or more inventories of the ICT assets. The inventory shall include hardware and software assets as well as the storage locations of critical data. Both dependencies within the institution as well as interfaces to significant external service providers should be taken into account.</t>
+  </si>
+  <si>
+    <t>The inventory is available in real time and shall be reviewed and updated regularly with regard to its completeness and accuracy.</t>
+  </si>
+  <si>
+    <t>The institution shall have procedures, processes and controls in place that ensure the confidentiality, integrity and availability of the ICT production environment, taking into account the respective risk tolerance.</t>
+  </si>
+  <si>
+    <t>The institution shall ensure that it can transition smoothly to its BCP and DRP processes in the event of significant disruptions to its ICT operations. It shall implement adequate back-up processes and recovery processes that are tested and validated regularly.</t>
+  </si>
+  <si>
+    <t>The institution shall have procedures, processes and controls in place to ensure that ICT that its nearing the end of its operational life or whose planned decommissioning date has passed is dealt with in a risk-oriented way.</t>
+  </si>
+  <si>
+    <t>d) Incident management</t>
+  </si>
+  <si>
+    <t>The institution shall have procedures, processes and controls in place for dealing with significant ICT incidents, including those resulting from dependencies on external service providers and outsourcing operations within the group. In this regard, the full life-cycle of significant ICT incidents must be taken into account and tasks, competencies and responsibilities for dealing with these incidents must be defined.</t>
+  </si>
+  <si>
+    <t>Dealing with significant ICT incidents must be coordinated and linked with the processes for BCM and the DRP.</t>
+  </si>
+  <si>
+    <t>ICT incidents that are regarded by the institution as a significant disruption in the provision of its critical processes and are of material significance for supervision must be reported to FINMA without delay.</t>
+  </si>
+  <si>
+    <t>C. Cyber risk management</t>
+  </si>
+  <si>
+    <t>The basic expectations for the strategy, governance and raising of awareness in relation to cyber risks are set out in margin nos. 23–26 and 40.</t>
+  </si>
+  <si>
+    <t>The institution shall define clear tasks, competencies and responsibilities. It must cover at least the following aspects in accordance with internationally recognised standards and practices, and ensure their effective implementation through appropriate procedures, processes and controls and continuously develop and improve them:</t>
+  </si>
+  <si>
+    <t>a. Identification of the institution-specific threat landscape from cyber attacks14 and assessment of the possible impacts of exploiting vulnerabilities with regard to the inventoried ICT assets and the electronic critical data (in accordance with margin nos. 53, 54 and 7);</t>
+  </si>
+  <si>
+    <t>[14] Attacks on the confidentiality, integrity and availability of ICT as well as the electronic critical data that take place as a result of external or internal attackers exploiting vulnerabilities or circumventing protective measures.</t>
+  </si>
+  <si>
+    <t>b. Protection of the inventoried ICT assets and the electronic critical data from cyber attacks by implementing appropriate protective measures, particularly with regard to the confidentiality, integrity and availability;</t>
+  </si>
+  <si>
+    <t>c. Timely logging and detection of cyber attacks on the basis of a process for the systematic and consistent monitoring of the inventoried ICT assets and the electronic critical data;</t>
+  </si>
+  <si>
+    <t>d. Response to identified vulnerabilities and cyber attacks by developing and implementing appropriate processes for taking rapid containment and remediation measures; and</t>
+  </si>
+  <si>
+    <t>e. Ensuring the prompt recovery of normal business operations after a cyber attack through appropriate measures.</t>
+  </si>
+  <si>
+    <t>Cyber risk management must ensure that a successful or partially successful cyber attack is analysed based on its materiality for critical inventoried ICT assets or electronic critical data and critical processes (including outsourced services and functions) and that the reporting obligation under the FINMASA is met. After an initial assessment and preliminary notification to the body responsible at FINMA within 24 hours, the report in accordance with the catalogue of requirements on the EHP survey and application platform (mandatory fields) must be submitted to FINMA within 72 hours. Once the institution has finished processing the case, a conclusive root cause analysis corresponding to the degree of severity must be submitted to the body responsible at FINMA.</t>
+  </si>
+  <si>
+    <t>The executive board shall arrange for vulnerability assessments15 and penetration tests16 to be conducted regularly. These must be performed by qualified staff with adequate resources. All inventoried ICT assets that are accessible over the internet must be taken into account. In addition, inventoried ICT assets that are not accessible over the internet, but that are necessary for the provision of critical processes, or that contain electronic critical data, must be included as well.</t>
+  </si>
+  <si>
+    <t>[15] Analysis used to identify existing software vulnerabilities and security gaps in the IT infrastructure towards cyber attacks.
+[16] Targeted audit and exploitation of software vulnerabilities and security gaps in the ICT.</t>
+  </si>
+  <si>
+    <t>Risk-based, threat intelligence-related scenario cyber exercises17 must be conducted on the basis of the institution-specific threat landscape. The result of the exercises must be documented and reported in an appropriate form.</t>
+  </si>
+  <si>
+    <t>[17] Taking into account margin no. 19, such cyber exercises may include, for example, tabletop, red team exercises etc.</t>
+  </si>
+  <si>
+    <t>D. Critical data risk management</t>
+  </si>
+  <si>
+    <t>The basic expectations for the strategy, governance and raising of awareness in relation to the risks of critical data are set out in margin nos. 23–26.</t>
+  </si>
+  <si>
+    <t>The executive board shall define appropriate processes, procedures and controls as well as clear tasks, competencies and responsibilities for dealing with the data identified as critical by the institution. Furthermore, the executive board shall appoint a unit to establish the framework for ensuring the confidentiality, integrity and availability of critical data and to monitor its observance.</t>
+  </si>
+  <si>
+    <t>The institution shall identify its critical data in a systematic and comprehensive way, categorise it on the basis of its criticality and define clear responsibilities.</t>
+  </si>
+  <si>
+    <t>The critical data defined by the institution must be managed throughout its entire lifecycle.</t>
+  </si>
+  <si>
+    <t>In the management of critical data, in particular the confidentiality, integrity and availability of the critical data must be ensured through appropriate processes, procedures and controls.</t>
+  </si>
+  <si>
+    <t>Critical data must be adequately protected from being accessed and used by unauthorised persons during operations and during the development, change and migration of ICT. This also applies to critical data in test environments.</t>
+  </si>
+  <si>
+    <t>The ICT assets that store or process critical data must be afforded particular protection. Access to these data must be regulated systematically and monitored continuously.</t>
+  </si>
+  <si>
+    <t>Access to critical data and processing functionalities shall be restricted to persons who require this to carry out their tasks18. The institution must have an authorisation system in place. Access to this authorisation system must be afforded particular protection and reviewed on a regular basis. The authorisations included in the authorisation system must be reviewed on a regular basis.</t>
+  </si>
+  <si>
+    <t>[18] For example, need-to-know and least privilege principles.</t>
+  </si>
+  <si>
+    <t>If critical data is stored outside of Switzerland19 or if it can be accessed from abroad, increased risks associated with this must be adequately mitigated and monitored via suitable means and the data afforded particular protection.</t>
+  </si>
+  <si>
+    <t>[19] For example, in the context of cloud or hosting solutions.</t>
+  </si>
+  <si>
+    <t>Both internal and external persons who can access critical data or who can change these must be selected carefully. These persons must be monitored with the help of appropriate measures20 and given regular training in the handling of these data. Increased security requirements shall apply to persons with increased privileges21. In addition, a list of all persons with privileged access rights must be kept and updated on a regular basis.</t>
+  </si>
+  <si>
+    <t>[20] For example, analysis of log files, “four eyes principle” etc.
+[21] For example, persons with administrator rights, users with functional access to a large quantity of critical data etc.</t>
+  </si>
+  <si>
+    <t>Incidents that substantially impair the confidentiality, integrity or availability of critical data must be reported to FINMA without delay.</t>
+  </si>
+  <si>
+    <t>When selecting service providers that can process22 or view critical data, due diligence must be particularly thorough. Clear criteria for assessing how service providers handle critical data must be defined and checked before entering into a contractual agreement. The service providers must be monitored and checked periodically as part of the institution’s internal control system.</t>
+  </si>
+  <si>
+    <t>[22] Processing: any handling of critical data, irrespective of the means and procedures used, in particular the collection, saving, storage, use, changing, disclosing, archiving, deletion or destruction of data.</t>
+  </si>
+  <si>
+    <t>The basic expectations for the strategy, governance and raising of awareness in relation to risks resulting from the design and implementation of BCM are set out in margin nos. 23–26.</t>
+  </si>
+  <si>
+    <t>Every relevant business and organisational area must identify its critical processes and the resources required for these23 in a business impact analysis (BIA).</t>
+  </si>
+  <si>
+    <t>[23] Staff, facilities (e.g. building, workplace infrastructure), information, IT systems or IT infrastructure (including communication systems), dependencies on other areas of the institution and on third parties, e.g. external service providers and suppliers (outsourcing), central banks or clearing houses.</t>
+  </si>
+  <si>
+    <t>The institution shall define the RTO and RPO for the critical processes in accordance with margin no. 10. These shall be coordinated with the necessary service providers24 and adherence to the RTO and RPO shall be regulated by service level agreements or contracts or by other appropriate procedures, processes and controls.</t>
+  </si>
+  <si>
+    <t>[24] For example, with the IT department, other units of the institution or external parties.</t>
+  </si>
+  <si>
+    <t>The institution shall define at least one BCP in accordance with margin no. 11 that also describes the conditions triggering the plan and the decision-making processes, and takes into account the loss of resources in accordance with margin no. 84. The acceptance of residual risks must be adequately documented.</t>
+  </si>
+  <si>
+    <t>The BIA and BCP shall be prepared and documented in a consistent manner following institution-wide guidelines. They must be reviewed and updated annually and on an ad hoc basis in the event of significant changes to the business operations (reorganisations, development of a new business segment etc.).</t>
+  </si>
+  <si>
+    <t>The institution shall define at least one DRP as part of the BCP. If critical processes or parts thereof are outsourced, the DRP shall take into account the external dependencies and contractual provisions as well as alternative solutions. The DRP must be reviewed and updated on an ad hoc basis in the event of significant changes and at least annually.</t>
+  </si>
+  <si>
+    <t>In crisis situations, a crisis unit shall take on the task of crisis management until order is restored. The conditions triggering a crisis and the tasks, competencies and responsibilities of the crisis unit must be regulated in advance and the crisis organisation aligned to the business activities and geographical structure of the institution. The availability of responsible persons in crisis situations must be ensured.</t>
+  </si>
+  <si>
+    <t>The institution shall define a communication strategy for internal and external communication in crisis situations.</t>
+  </si>
+  <si>
+    <t>The implementation of the BCP and DRP as well as the functioning of the crisis organisation must be regularly evaluated through tests. Systematic plans shall be drawn up for this, which ensure regular coverage. Various means of testing of varying intensity and effectiveness can be selected including, for example, tabletop exercises.</t>
+  </si>
+  <si>
+    <t>The most important measures according to the BCP and DRP and the crisis organisation must be tested at least once a year.</t>
+  </si>
+  <si>
+    <t>Relevant stakeholder groups, including those in specialist and IT functions, shall take part in the tests in order to familiarise themselves with the recovery processes.</t>
+  </si>
+  <si>
+    <t>The tests shall encompass various severe but plausible scenarios and take into account recovery dependencies, including those that exist with internal or external third parties.</t>
+  </si>
+  <si>
+    <t>Regular reporting to the board of directors and the executive board shall include information about the testing and review activities carried out and their results. It shall clearly show prioritisations made (e.g. prioritisation of the critical processes necessary for the provision of the critical functions in accordance with margin no. 14) and recognised gaps in the coverage of other critical processes.</t>
+  </si>
+  <si>
+    <t>The employees and members of the crisis organisation shall be adequately trained in their tasks, competencies and responsibilities resulting from the various BCM activities, both when new employees join the institution and as part of regular training.</t>
+  </si>
+  <si>
+    <t>F. Management of risks from cross-border service business</t>
+  </si>
+  <si>
+    <t>If institutions or their group companies provide services or distribute financial products cross-border, then the risks resulting from the application of foreign legislation (tax, criminal, anti-money laundering legislation etc.) must also be adequately identified, limited and controlled.</t>
+  </si>
+  <si>
+    <t>The institutions shall conduct a thorough analysis of their cross-border service business and cross-border distribution of financial products, examining the legal framework and associated risks. Based on this analysis, the institutions shall take the necessary strategic and organisational measures to eliminate and minimise risk, and continuously adapt these to changing conditions. In particular, they shall have the necessary country-specific specialist knowledge, define specific service models for the countries served, train employees and ensure compliance with the guidelines through appropriate organisational measures, directives, remuneration and sanctions models.</t>
+  </si>
+  <si>
+    <t>The risks generated by external asset managers, intermediaries and other service providers must also be taken into account. Accordingly, a diligent approach must be adopted in selecting and instructing these partners.</t>
+  </si>
+  <si>
+    <t>This basic approach also covers situations where a foreign-based subsidiary, branch or similar serves clients of a Swiss financial institution cross-border.</t>
+  </si>
+  <si>
+    <t>V. Ensuring operational resilience</t>
+  </si>
+  <si>
+    <t>The institution shall identify its critical functions and their tolerances for disruption. These must be approved by the board of directors. The board of directors must also regularly approve and monitor the approach for ensuring operational resilience.</t>
+  </si>
+  <si>
+    <t>The institution shall take measures to ensure operational resilience, taking into account severe but plausible scenarios25.</t>
+  </si>
+  <si>
+    <t>[25] It cannot be ruled out that some scenarios cannot be managed without state involvement (e.g. pandemics, wars, long-term power shortages). For such scenarios, preliminary work must be carried out by the institution for the purpose of strengthening its operational resilience to these scenarios in so far as its means allow.</t>
+  </si>
+  <si>
+    <t>The critical functions and the associated tolerances for disruption according to margin no. 14 must be approved at least annually by the board of directors.</t>
+  </si>
+  <si>
+    <t>The institution shall coordinate the relevant components of a comprehensive risk management framework, such as operational risk management, including ICT and cyber risk management, business continuity management, outsourcing management (cf. FINMA Circular 2018/3 “Outsourcing”), and emergency planning (Chapter VI.) such that these contribute to strengthening the institution’s operational resilience. This includes an appropriate exchange of relevant information between these various areas.</t>
+  </si>
+  <si>
+    <t>Reporting to the board of directors and the executive board must take place annually and in the event of significant control weaknesses or incidents that jeopardise operational resilience.</t>
+  </si>
+  <si>
+    <t>Internal and external threats and the corresponding exploitation of vulnerabilities shall be identified and assessed for the critical functions. The resulting operational risks shall be identified, assessed, limited and monitored as part of operational risk management.</t>
+  </si>
+  <si>
+    <t>The institution shall keep an inventory of its critical functions, which is reviewed and updated at least annually. This inventory shall contain the tolerances for disruption of the critical functions, as well as connections and dependencies between the necessary critical processes and their resources26 for providing the critical functions.</t>
+  </si>
+  <si>
+    <t>[26] Including the ICT assets of the inventory in accordance with margin no. 53 relevant to the critical functions.</t>
+  </si>
+  <si>
+    <t>As a minimum, the significant operational risks and the key controls must be documented for the critical functions.</t>
+  </si>
+  <si>
+    <t>The critical functions and the critical processes and resources required for these shall be covered by BCPs pursuant to Chapter IV./E.</t>
+  </si>
+  <si>
+    <t>The ability to provide critical functions within their tolerance for disruption in severe but plausible scenarios shall be tested or exercised regularly. These also include scenarios that differ from shorter and more limited interruptions and that are characterised by a longer duration (e.g. over several months) and a lack of basic resources27. The tests or exercises must be designed in such a way that they do not fundamentally endanger the institution.</t>
+  </si>
+  <si>
+    <t>[27] Examples include a pandemic, a power shortage, a prolonged downtime resulting from the insolvency of a key service provider (as an example of a stressed exit by a service provider) or a long-term prohibition of foreign governments, according to which foreign-based cloud providers or other service providers are no longer permitted to serve Swiss firms.</t>
+  </si>
+  <si>
+    <t>For systemically important banks, the BCP, DRP and the crisis organisation in accordance with Chapter IV./E. that are relevant for the continuation of the critical functions in accordance with margin no. 14 must be coordinated with the emergency planning in accordance with Chapter VI.</t>
+  </si>
+  <si>
+    <t>VI. Continuation of critical services during the resolution and recovery of systemically important banks</t>
+  </si>
+  <si>
+    <t>As part of their emergency planning, systemically important banks shall take the necessary measures for the uninterrupted continuation of systemically important functions (Art. 9 para. 2 let. d BA in conjunction with Art. 60 ff. BO). They shall identify the services necessary to continue the systemically important functions in the event of resolution, recovery or restructuring (“critical services”) and take the measures necessary for their continuation. In doing so they shall take into account the requirements issued by international standard setters in this context.</t>
+  </si>
+  <si>
+    <t>VII. Transitional provisions</t>
+  </si>
+  <si>
+    <t>A. Concerning ensuring operational resilience</t>
+  </si>
+  <si>
+    <t>The identification of critical functions, the definition of tolerances for disruption and initial approvals in accordance with margin nos. 101 and 103, as well as initial reporting in accordance with margin no. 105, will be expected following the Circular’s entry into force. A transitional period of one year from the entry into force shall apply for fulfilling the requirements in accordance with margin nos. 106–109 and the first tests in accordance with margin no. 110. It is expected that operational resilience will be ensured in accordance with margin no. 102 and the requirements met in accordance with margin nos. 104 and 111 within a transitional period of two years.</t>
+  </si>
+  <si>
+    <t>B. Concerning the capital requirements for operational risk</t>
+  </si>
+  <si>
+    <t>The capital requirements for operational risk in accordance with Article 89 ff. CAO shall be based on margin nos. 3–116 of FINMA Circular 2008/21 “Operational risk – banks” until the entry into force of the CAO revised as part of the final Basel III revision package and the implementing FINMA ordinance.</t>
+  </si>
+  <si>
+    <t>2025-06-10</t>
+  </si>
+  <si>
+    <t>FINMA - Circular 2023/01 - Operational risks and resilience - Banks</t>
+  </si>
+  <si>
+    <t>Managing operational risks and ensuring operational resilience
+Reference: FINMA Circ. 23/1 “Operational risks and resilience – banks”
+Date: 7 December 2022
+Entry into force: 1 January 2024
+Concordance: former FINMA Circ. 08/21 “Operational risk – banks”, dated 20 November 2008
+Legal framework: FINMASA Articles 7 para. 1 let. b and 29 para. 1
+                                 BA Article 1b para. 3 let. b, Articles 3 para. 2 let. a and 3f
+                                 BO Articles 12 and 14e
+                                 FinIA Articles 9 and 49
+                                 FinIO Articles 12 and 68</t>
+  </si>
+  <si>
+    <t>Margin no. 1</t>
+  </si>
+  <si>
+    <t>Margin no. 2</t>
+  </si>
+  <si>
+    <t>Margin no. 3</t>
+  </si>
+  <si>
+    <t>Margin no. 4</t>
+  </si>
+  <si>
+    <t>Margin no. 5</t>
+  </si>
+  <si>
+    <t>Margin no. 6</t>
+  </si>
+  <si>
+    <t>Margin no. 7</t>
+  </si>
+  <si>
+    <t>Margin no. 8</t>
+  </si>
+  <si>
+    <t>Margin no. 9</t>
+  </si>
+  <si>
+    <t>Margin no. 10</t>
+  </si>
+  <si>
+    <t>Margin no. 11</t>
+  </si>
+  <si>
+    <t>Margin no. 12</t>
+  </si>
+  <si>
+    <t>Margin no. 13</t>
+  </si>
+  <si>
+    <t>Margin no. 14</t>
+  </si>
+  <si>
+    <t>Margin no. 15</t>
+  </si>
+  <si>
+    <t>Margin no. 16</t>
+  </si>
+  <si>
+    <t>Margin no. 17</t>
+  </si>
+  <si>
+    <t>Margin no. 18</t>
+  </si>
+  <si>
+    <t>Margin no. 19</t>
+  </si>
+  <si>
+    <t>Margin no. 20</t>
+  </si>
+  <si>
+    <t>Margin no. 21</t>
+  </si>
+  <si>
+    <t>Margin no. 22</t>
+  </si>
+  <si>
+    <t>Margin no. 23</t>
+  </si>
+  <si>
+    <t>Margin no. 24</t>
+  </si>
+  <si>
+    <t>Margin no. 25</t>
+  </si>
+  <si>
+    <t>Margin no. 26</t>
+  </si>
+  <si>
+    <t>Margin no. 27</t>
+  </si>
+  <si>
+    <t>Margin no. 28</t>
+  </si>
+  <si>
+    <t>Margin no. 29</t>
+  </si>
+  <si>
+    <t>Margin no. 30</t>
+  </si>
+  <si>
+    <t>Margin no. 31</t>
+  </si>
+  <si>
+    <t>Margin no. 32</t>
+  </si>
+  <si>
+    <t>Margin no. 33</t>
+  </si>
+  <si>
+    <t>Margin no. 34</t>
+  </si>
+  <si>
+    <t>Margin no. 35</t>
+  </si>
+  <si>
+    <t>Margin no. 36</t>
+  </si>
+  <si>
+    <t>Margin no. 37</t>
+  </si>
+  <si>
+    <t>Margin no. 38</t>
+  </si>
+  <si>
+    <t>Margin no. 39</t>
+  </si>
+  <si>
+    <t>Margin no. 40</t>
+  </si>
+  <si>
+    <t>Margin no. 41</t>
+  </si>
+  <si>
+    <t>Margin no. 42</t>
+  </si>
+  <si>
+    <t>Margin no. 43</t>
+  </si>
+  <si>
+    <t>Margin no. 44</t>
+  </si>
+  <si>
+    <t>Margin no. 45</t>
+  </si>
+  <si>
+    <t>Margin no. 46</t>
+  </si>
+  <si>
+    <t>Margin no. 47</t>
+  </si>
+  <si>
+    <t>Margin no. 48</t>
+  </si>
+  <si>
+    <t>Margin no. 49</t>
+  </si>
+  <si>
+    <t>Margin no. 50</t>
+  </si>
+  <si>
+    <t>Margin no. 51</t>
+  </si>
+  <si>
+    <t>Margin no. 52</t>
+  </si>
+  <si>
+    <t>Margin no. 53</t>
+  </si>
+  <si>
+    <t>Margin no. 54</t>
+  </si>
+  <si>
+    <t>Margin no. 55</t>
+  </si>
+  <si>
+    <t>Margin no. 56</t>
+  </si>
+  <si>
+    <t>Margin no. 57</t>
+  </si>
+  <si>
+    <t>Margin no. 58</t>
+  </si>
+  <si>
+    <t>Margin no. 59</t>
+  </si>
+  <si>
+    <t>Margin no. 60</t>
+  </si>
+  <si>
+    <t>Margin no. 61</t>
+  </si>
+  <si>
+    <t>Margin no. 62</t>
+  </si>
+  <si>
+    <t>Margin no. 63</t>
+  </si>
+  <si>
+    <t>Margin no. 64</t>
+  </si>
+  <si>
+    <t>Margin no. 65</t>
+  </si>
+  <si>
+    <t>Margin no. 66</t>
+  </si>
+  <si>
+    <t>Margin no. 67</t>
+  </si>
+  <si>
+    <t>Margin no. 68</t>
+  </si>
+  <si>
+    <t>Margin no. 69</t>
+  </si>
+  <si>
+    <t>Margin no. 70</t>
+  </si>
+  <si>
+    <t>Margin no. 71</t>
+  </si>
+  <si>
+    <t>Margin no. 72</t>
+  </si>
+  <si>
+    <t>Margin no. 73</t>
+  </si>
+  <si>
+    <t>Margin no. 74</t>
+  </si>
+  <si>
+    <t>Margin no. 75</t>
+  </si>
+  <si>
+    <t>Margin no. 76</t>
+  </si>
+  <si>
+    <t>Margin no. 77</t>
+  </si>
+  <si>
+    <t>Margin no. 78</t>
+  </si>
+  <si>
+    <t>Margin no. 79</t>
+  </si>
+  <si>
+    <t>Margin no. 80</t>
+  </si>
+  <si>
+    <t>Margin no. 81</t>
+  </si>
+  <si>
+    <t>Margin no. 82</t>
+  </si>
+  <si>
+    <t>Margin no. 83</t>
+  </si>
+  <si>
+    <t>Margin no. 84</t>
+  </si>
+  <si>
+    <t>Margin no. 85</t>
+  </si>
+  <si>
+    <t>Margin no. 86</t>
+  </si>
+  <si>
+    <t>Margin no. 87</t>
+  </si>
+  <si>
+    <t>Margin no. 88</t>
+  </si>
+  <si>
+    <t>Margin no. 89</t>
+  </si>
+  <si>
+    <t>Margin no. 90</t>
+  </si>
+  <si>
+    <t>Margin no. 91</t>
+  </si>
+  <si>
+    <t>Margin no. 92</t>
+  </si>
+  <si>
+    <t>Margin no. 93</t>
+  </si>
+  <si>
+    <t>Margin no. 94</t>
+  </si>
+  <si>
+    <t>Margin no. 95</t>
+  </si>
+  <si>
+    <t>Margin no. 96</t>
+  </si>
+  <si>
+    <t>Margin no. 97</t>
+  </si>
+  <si>
+    <t>Margin no. 98</t>
+  </si>
+  <si>
+    <t>Margin no. 99</t>
+  </si>
+  <si>
+    <t>Margin no. 100</t>
+  </si>
+  <si>
+    <t>Margin no. 101</t>
+  </si>
+  <si>
+    <t>Margin no. 102</t>
+  </si>
+  <si>
+    <t>Margin no. 103</t>
+  </si>
+  <si>
+    <t>Margin no. 104</t>
+  </si>
+  <si>
+    <t>Margin no. 105</t>
+  </si>
+  <si>
+    <t>Margin no. 106</t>
+  </si>
+  <si>
+    <t>Margin no. 107</t>
+  </si>
+  <si>
+    <t>Margin no. 108</t>
+  </si>
+  <si>
+    <t>Margin no. 109</t>
+  </si>
+  <si>
+    <t>Margin no. 110</t>
+  </si>
+  <si>
+    <t>Margin no. 111</t>
+  </si>
+  <si>
+    <t>Margin no. 112</t>
+  </si>
+  <si>
+    <t>Margin no. 113</t>
+  </si>
+  <si>
+    <t>Margin no. 114</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -971,11 +1813,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1278,16 +2123,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="95.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1295,7 +2143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1303,7 +2151,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1311,7 +2159,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -1319,7 +2167,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1327,7 +2175,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -1335,7 +2183,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -1343,36 +2191,53 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
+        <v>299</v>
+      </c>
+      <c r="B8" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>300</v>
+      </c>
+      <c r="B9" t="s">
+        <v>459</v>
+      </c>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B10" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B12" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>19</v>
       </c>
-      <c r="B11" t="s">
-        <v>20</v>
+      <c r="B13" s="2" t="s">
+        <v>457</v>
       </c>
     </row>
   </sheetData>
@@ -1382,40 +2247,42 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:XFD8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>22</v>
       </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1423,7 +2290,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1431,13 +2298,30 @@
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>299</v>
+      </c>
+      <c r="B7" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>300</v>
+      </c>
+      <c r="B8" t="s">
+        <v>459</v>
+      </c>
+      <c r="C8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1446,24 +2330,28 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:F134"/>
+  <dimension ref="A1:I134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A121" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H134" sqref="H134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="114.88671875" customWidth="1"/>
     <col min="6" max="6" width="75.33203125" customWidth="1"/>
+    <col min="7" max="7" width="20.109375" customWidth="1"/>
+    <col min="8" max="8" width="142" style="1" customWidth="1"/>
+    <col min="9" max="9" width="78.21875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" t="s">
         <v>25</v>
-      </c>
-      <c r="B1" t="s">
-        <v>26</v>
       </c>
       <c r="C1" t="s">
         <v>8</v>
@@ -1475,1892 +2363,2713 @@
         <v>12</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
+        <v>299</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>300</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="G2" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="G3" t="s">
+        <v>460</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>33</v>
-      </c>
       <c r="F4" s="1"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G4" t="s">
+        <v>461</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="G5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G6" t="s">
+        <v>462</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="F7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G7" t="s">
+        <v>463</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>2</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="F8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G8" t="s">
+        <v>464</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>2</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>43</v>
-      </c>
       <c r="F9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="G9" t="s">
+        <v>465</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="F10" s="1"/>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G10" t="s">
+        <v>466</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>2</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>47</v>
-      </c>
       <c r="F11" s="1"/>
-    </row>
-    <row r="12" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G11" t="s">
+        <v>467</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>2</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
+        <v>47</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="F12" s="1"/>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G12" t="s">
+        <v>468</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>2</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="F13" s="1"/>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G13" t="s">
+        <v>469</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>2</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="E14" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="F14" s="1"/>
-    </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G14" t="s">
+        <v>470</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>2</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
+        <v>53</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="E15" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="F15" s="1"/>
-    </row>
-    <row r="16" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="G15" t="s">
+        <v>471</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>2</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>57</v>
-      </c>
       <c r="F16" s="1"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G16" t="s">
+        <v>472</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>2</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
+        <v>57</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="E17" s="1" t="s">
-        <v>59</v>
-      </c>
       <c r="F17" s="1"/>
-    </row>
-    <row r="18" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G17" t="s">
+        <v>473</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="E18" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="F18" s="1"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G18" t="s">
+        <v>474</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>2</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
+        <v>61</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="1" t="s">
-        <v>63</v>
-      </c>
       <c r="F19" s="1"/>
-    </row>
-    <row r="20" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G19" t="s">
+        <v>475</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>2</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="E20" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="F20" s="1"/>
-    </row>
-    <row r="21" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="G20" t="s">
+        <v>476</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>2</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
+        <v>65</v>
+      </c>
+      <c r="E21" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G21" t="s">
+        <v>477</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>323</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
-    </row>
-    <row r="23" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G22" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>2</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
+        <v>69</v>
+      </c>
+      <c r="E23" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="F23" s="1"/>
-    </row>
-    <row r="24" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G23" t="s">
+        <v>478</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>2</v>
       </c>
-      <c r="C24" t="s">
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="E24" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="F24" s="1"/>
-    </row>
-    <row r="25" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G24" t="s">
+        <v>479</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>2</v>
       </c>
-      <c r="C25" t="s">
+      <c r="D25" t="s">
+        <v>73</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>75</v>
-      </c>
       <c r="F25" s="1"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G25" t="s">
+        <v>480</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G26" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>2</v>
       </c>
       <c r="D27" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
-    </row>
-    <row r="28" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G27" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>3</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
+        <v>77</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="1" t="s">
-        <v>79</v>
-      </c>
       <c r="F28" s="1"/>
-    </row>
-    <row r="29" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="G28" t="s">
+        <v>481</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="D29" t="s">
         <v>80</v>
       </c>
-      <c r="B29">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="E29" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="F29" s="1" t="s">
+      <c r="G29" t="s">
+        <v>482</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>332</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>79</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="D30" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30">
-        <v>3</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="E30" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1"/>
+      <c r="G30" t="s">
+        <v>483</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="D31" t="s">
         <v>85</v>
       </c>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>80</v>
-      </c>
-      <c r="B31">
-        <v>3</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="E31" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F31" s="1" t="s">
+      <c r="G31" t="s">
+        <v>484</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>335</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>79</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="D32" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>80</v>
-      </c>
-      <c r="B32">
-        <v>3</v>
-      </c>
-      <c r="C32" t="s">
+      <c r="E32" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="F32" s="1" t="s">
+      <c r="G32" t="s">
+        <v>485</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>337</v>
+      </c>
+      <c r="I32" s="1" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>79</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>80</v>
-      </c>
-      <c r="B33">
-        <v>3</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="E33" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1"/>
+      <c r="G33" t="s">
+        <v>486</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>79</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="D34" t="s">
         <v>93</v>
       </c>
-      <c r="F33" s="1"/>
-    </row>
-    <row r="34" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>80</v>
-      </c>
-      <c r="B34">
-        <v>3</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="E34" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1"/>
+      <c r="G34" t="s">
+        <v>487</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="D35" t="s">
         <v>95</v>
       </c>
-      <c r="F34" s="1"/>
-    </row>
-    <row r="35" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>80</v>
-      </c>
-      <c r="B35">
-        <v>3</v>
-      </c>
-      <c r="C35" t="s">
+      <c r="E35" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="F35" s="1" t="s">
+      <c r="G35" t="s">
+        <v>488</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>79</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>80</v>
-      </c>
-      <c r="B36">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
+      <c r="E36" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F36" s="1" t="s">
+      <c r="G36" t="s">
+        <v>489</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>79</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="D37" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>80</v>
-      </c>
-      <c r="B37">
-        <v>3</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="E37" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1"/>
+      <c r="G37" t="s">
+        <v>490</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>79</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="D38" t="s">
         <v>103</v>
       </c>
-      <c r="F37" s="1"/>
-    </row>
-    <row r="38" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>80</v>
-      </c>
-      <c r="B38">
-        <v>3</v>
-      </c>
-      <c r="C38" t="s">
+      <c r="E38" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1"/>
+      <c r="G38" t="s">
+        <v>491</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>79</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="D39" t="s">
         <v>105</v>
       </c>
-      <c r="F38" s="1"/>
-    </row>
-    <row r="39" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>80</v>
-      </c>
-      <c r="B39">
-        <v>3</v>
-      </c>
-      <c r="C39" t="s">
+      <c r="E39" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="E39" s="1" t="s">
+      <c r="F39" s="1"/>
+      <c r="G39" t="s">
+        <v>492</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>79</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="D40" t="s">
         <v>107</v>
       </c>
-      <c r="F39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>80</v>
-      </c>
-      <c r="B40">
-        <v>3</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="E40" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E40" s="1" t="s">
+      <c r="F40" s="1"/>
+      <c r="G40" t="s">
+        <v>493</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>79</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="D41" t="s">
         <v>109</v>
       </c>
-      <c r="F40" s="1"/>
-    </row>
-    <row r="41" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>80</v>
-      </c>
-      <c r="B41">
-        <v>3</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="E41" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="F41" s="1"/>
+      <c r="G41" t="s">
+        <v>494</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="D42" t="s">
         <v>111</v>
       </c>
-      <c r="F41" s="1"/>
-    </row>
-    <row r="42" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>80</v>
-      </c>
-      <c r="B42">
-        <v>3</v>
-      </c>
-      <c r="C42" t="s">
+      <c r="E42" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="F42" s="1"/>
+      <c r="G42" t="s">
+        <v>495</v>
+      </c>
+      <c r="H42" s="1" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>79</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="D43" t="s">
         <v>113</v>
       </c>
-      <c r="F42" s="1"/>
-    </row>
-    <row r="43" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>80</v>
-      </c>
-      <c r="B43">
-        <v>3</v>
-      </c>
-      <c r="C43" t="s">
+      <c r="E43" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="E43" s="1" t="s">
+      <c r="F43" s="1"/>
+      <c r="G43" t="s">
+        <v>496</v>
+      </c>
+      <c r="H43" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>79</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="D44" t="s">
         <v>115</v>
       </c>
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>80</v>
-      </c>
-      <c r="B44">
-        <v>3</v>
-      </c>
-      <c r="C44" t="s">
+      <c r="E44" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="E44" s="1" t="s">
+      <c r="F44" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="F44" s="1" t="s">
+      <c r="G44" t="s">
+        <v>497</v>
+      </c>
+      <c r="H44" s="1" t="s">
+        <v>352</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>79</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="D45" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>80</v>
-      </c>
-      <c r="B45">
-        <v>3</v>
-      </c>
-      <c r="C45" t="s">
+      <c r="E45" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="E45" s="1" t="s">
+      <c r="F45" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="F45" s="1" t="s">
+      <c r="G45" t="s">
+        <v>498</v>
+      </c>
+      <c r="H45" s="1" t="s">
+        <v>354</v>
+      </c>
+      <c r="I45" s="1" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>79</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="D46" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>80</v>
-      </c>
-      <c r="B46">
-        <v>3</v>
-      </c>
-      <c r="C46" t="s">
+      <c r="E46" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E46" s="1" t="s">
+      <c r="F46" s="1"/>
+      <c r="G46" t="s">
+        <v>499</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="D47" t="s">
         <v>123</v>
       </c>
-      <c r="F46" s="1"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>80</v>
-      </c>
-      <c r="B47">
-        <v>3</v>
-      </c>
-      <c r="C47" t="s">
+      <c r="E47" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="E47" s="1" t="s">
+      <c r="F47" s="1"/>
+      <c r="G47" t="s">
+        <v>500</v>
+      </c>
+      <c r="H47" s="1" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>79</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="D48" t="s">
         <v>125</v>
       </c>
-      <c r="F47" s="1"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>80</v>
-      </c>
-      <c r="B48">
-        <v>3</v>
-      </c>
-      <c r="C48" t="s">
+      <c r="E48" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="E48" s="1" t="s">
+      <c r="F48" s="1"/>
+      <c r="G48" t="s">
+        <v>501</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>79</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="D49" t="s">
         <v>127</v>
       </c>
-      <c r="F48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
-        <v>80</v>
-      </c>
-      <c r="B49">
-        <v>3</v>
-      </c>
-      <c r="C49" t="s">
+      <c r="E49" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E49" s="1" t="s">
+      <c r="F49" s="1"/>
+      <c r="G49" t="s">
+        <v>502</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>79</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="D50" t="s">
         <v>129</v>
       </c>
-      <c r="F49" s="1"/>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A50" t="s">
-        <v>80</v>
-      </c>
-      <c r="B50">
-        <v>3</v>
-      </c>
-      <c r="C50" t="s">
+      <c r="E50" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E50" s="1" t="s">
+      <c r="F50" s="1"/>
+      <c r="G50" t="s">
+        <v>503</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>79</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="D51" t="s">
         <v>131</v>
       </c>
-      <c r="F50" s="1"/>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A51" t="s">
-        <v>80</v>
-      </c>
-      <c r="B51">
-        <v>3</v>
-      </c>
-      <c r="C51" t="s">
+      <c r="E51" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E51" s="1" t="s">
+      <c r="F51" s="1"/>
+      <c r="G51" t="s">
+        <v>504</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>79</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="D52" t="s">
         <v>133</v>
       </c>
-      <c r="F51" s="1"/>
-    </row>
-    <row r="52" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52" t="s">
-        <v>80</v>
-      </c>
-      <c r="B52">
-        <v>3</v>
-      </c>
-      <c r="C52" t="s">
+      <c r="E52" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E52" s="1" t="s">
-        <v>135</v>
-      </c>
       <c r="F52" s="1"/>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G52" t="s">
+        <v>505</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B53">
         <v>2</v>
       </c>
       <c r="D53" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G53" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B54">
         <v>3</v>
       </c>
       <c r="D54" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G54" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B55">
         <v>4</v>
       </c>
-      <c r="C55" t="s">
+      <c r="D55" t="s">
+        <v>137</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="F55" s="1"/>
-    </row>
-    <row r="56" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G55" t="s">
+        <v>506</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B56">
         <v>4</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
+        <v>139</v>
+      </c>
+      <c r="E56" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E56" s="1" t="s">
-        <v>141</v>
-      </c>
       <c r="F56" s="1"/>
-    </row>
-    <row r="57" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G56" t="s">
+        <v>507</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B57">
         <v>4</v>
       </c>
-      <c r="C57" t="s">
+      <c r="D57" t="s">
+        <v>141</v>
+      </c>
+      <c r="E57" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="E57" s="1" t="s">
-        <v>143</v>
-      </c>
       <c r="F57" s="1"/>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G57" t="s">
+        <v>508</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B58">
         <v>3</v>
       </c>
       <c r="D58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
-    </row>
-    <row r="59" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G58" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B59">
         <v>4</v>
       </c>
-      <c r="C59" t="s">
-        <v>144</v>
+      <c r="D59" t="s">
+        <v>143</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F59" s="1"/>
-    </row>
-    <row r="60" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G59" t="s">
+        <v>509</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B60">
         <v>4</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
+        <v>146</v>
+      </c>
+      <c r="E60" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="E60" s="1" t="s">
-        <v>148</v>
-      </c>
       <c r="F60" s="1"/>
-    </row>
-    <row r="61" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G60" t="s">
+        <v>510</v>
+      </c>
+      <c r="H60" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B61">
         <v>4</v>
       </c>
-      <c r="C61" t="s">
+      <c r="D61" t="s">
+        <v>148</v>
+      </c>
+      <c r="E61" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="E61" s="1" t="s">
+      <c r="F61" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="F61" s="1" t="s">
+      <c r="G61" t="s">
+        <v>511</v>
+      </c>
+      <c r="H61" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <v>3</v>
+      </c>
+      <c r="D62" t="s">
         <v>151</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B62">
-        <v>3</v>
-      </c>
-      <c r="D62" t="s">
-        <v>152</v>
       </c>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
-    </row>
-    <row r="63" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G62" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B63">
         <v>4</v>
       </c>
-      <c r="C63" t="s">
+      <c r="D63" t="s">
+        <v>152</v>
+      </c>
+      <c r="E63" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E63" s="1" t="s">
-        <v>154</v>
-      </c>
       <c r="F63" s="1"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G63" t="s">
+        <v>512</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B64">
         <v>4</v>
       </c>
-      <c r="C64" t="s">
+      <c r="D64" t="s">
+        <v>154</v>
+      </c>
+      <c r="E64" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E64" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="F64" s="1"/>
-    </row>
-    <row r="65" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G64" t="s">
+        <v>513</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B65">
         <v>4</v>
       </c>
-      <c r="C65" t="s">
+      <c r="D65" t="s">
+        <v>156</v>
+      </c>
+      <c r="E65" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="E65" s="1" t="s">
-        <v>158</v>
-      </c>
       <c r="F65" s="1"/>
-    </row>
-    <row r="66" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G65" t="s">
+        <v>514</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B66">
         <v>4</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
+        <v>158</v>
+      </c>
+      <c r="E66" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="E66" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="F66" s="1"/>
-    </row>
-    <row r="67" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G66" t="s">
+        <v>515</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B67">
         <v>4</v>
       </c>
-      <c r="C67" t="s">
+      <c r="D67" t="s">
+        <v>160</v>
+      </c>
+      <c r="E67" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="E67" s="1" t="s">
+      <c r="F67" s="1"/>
+      <c r="G67" t="s">
+        <v>516</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>3</v>
+      </c>
+      <c r="D68" t="s">
         <v>162</v>
-      </c>
-      <c r="F67" s="1"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="B68">
-        <v>3</v>
-      </c>
-      <c r="D68" t="s">
-        <v>163</v>
       </c>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
-    </row>
-    <row r="69" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G68" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B69">
         <v>4</v>
       </c>
-      <c r="C69" t="s">
+      <c r="D69" t="s">
+        <v>163</v>
+      </c>
+      <c r="E69" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E69" s="1" t="s">
-        <v>165</v>
-      </c>
       <c r="F69" s="1"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G69" t="s">
+        <v>517</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B70">
         <v>4</v>
       </c>
-      <c r="C70" t="s">
+      <c r="D70" t="s">
+        <v>165</v>
+      </c>
+      <c r="E70" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E70" s="1" t="s">
-        <v>167</v>
-      </c>
       <c r="F70" s="1"/>
-    </row>
-    <row r="71" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G70" t="s">
+        <v>518</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B71">
         <v>4</v>
       </c>
-      <c r="C71" t="s">
+      <c r="D71" t="s">
+        <v>167</v>
+      </c>
+      <c r="E71" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E71" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="F71" s="1"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G71" t="s">
+        <v>519</v>
+      </c>
+      <c r="H71" s="1" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B72">
         <v>2</v>
       </c>
       <c r="D72" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
-    </row>
-    <row r="73" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G72" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B73">
         <v>3</v>
       </c>
-      <c r="C73" t="s">
+      <c r="D73" t="s">
+        <v>170</v>
+      </c>
+      <c r="E73" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="E73" s="1" t="s">
+      <c r="F73" s="1"/>
+      <c r="G73" t="s">
+        <v>520</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>79</v>
+      </c>
+      <c r="B74">
+        <v>3</v>
+      </c>
+      <c r="D74" t="s">
         <v>172</v>
       </c>
-      <c r="F73" s="1"/>
-    </row>
-    <row r="74" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>80</v>
-      </c>
-      <c r="B74">
-        <v>3</v>
-      </c>
-      <c r="C74" t="s">
+      <c r="E74" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E74" s="1" t="s">
+      <c r="F74" s="1"/>
+      <c r="G74" t="s">
+        <v>521</v>
+      </c>
+      <c r="H74" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>79</v>
+      </c>
+      <c r="B75">
+        <v>3</v>
+      </c>
+      <c r="D75" t="s">
         <v>174</v>
       </c>
-      <c r="F74" s="1"/>
-    </row>
-    <row r="75" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>80</v>
-      </c>
-      <c r="B75">
-        <v>3</v>
-      </c>
-      <c r="C75" t="s">
+      <c r="E75" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E75" s="1" t="s">
+      <c r="F75" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F75" s="1" t="s">
+      <c r="G75" t="s">
+        <v>522</v>
+      </c>
+      <c r="H75" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="I75" s="1" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>79</v>
+      </c>
+      <c r="B76">
+        <v>3</v>
+      </c>
+      <c r="D76" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>80</v>
-      </c>
-      <c r="B76">
-        <v>3</v>
-      </c>
-      <c r="C76" t="s">
+      <c r="E76" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E76" s="1" t="s">
+      <c r="F76" s="1"/>
+      <c r="G76" t="s">
+        <v>523</v>
+      </c>
+      <c r="H76" s="1" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>79</v>
+      </c>
+      <c r="B77">
+        <v>3</v>
+      </c>
+      <c r="D77" t="s">
         <v>179</v>
       </c>
-      <c r="F76" s="1"/>
-    </row>
-    <row r="77" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>80</v>
-      </c>
-      <c r="B77">
-        <v>3</v>
-      </c>
-      <c r="C77" t="s">
+      <c r="E77" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="F77" s="1"/>
+      <c r="G77" t="s">
+        <v>524</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78">
+        <v>3</v>
+      </c>
+      <c r="D78" t="s">
         <v>181</v>
       </c>
-      <c r="F77" s="1"/>
-    </row>
-    <row r="78" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>80</v>
-      </c>
-      <c r="B78">
-        <v>3</v>
-      </c>
-      <c r="C78" t="s">
+      <c r="E78" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="E78" s="1" t="s">
+      <c r="F78" s="1"/>
+      <c r="G78" t="s">
+        <v>525</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79">
+        <v>3</v>
+      </c>
+      <c r="D79" t="s">
         <v>183</v>
       </c>
-      <c r="F78" s="1"/>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>80</v>
-      </c>
-      <c r="B79">
-        <v>3</v>
-      </c>
-      <c r="C79" t="s">
+      <c r="E79" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E79" s="1" t="s">
+      <c r="F79" s="1"/>
+      <c r="G79" t="s">
+        <v>526</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>3</v>
+      </c>
+      <c r="D80" t="s">
         <v>185</v>
       </c>
-      <c r="F79" s="1"/>
-    </row>
-    <row r="80" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>80</v>
-      </c>
-      <c r="B80">
-        <v>3</v>
-      </c>
-      <c r="C80" t="s">
+      <c r="E80" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="F80" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="F80" s="1" t="s">
+      <c r="G80" t="s">
+        <v>527</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>3</v>
+      </c>
+      <c r="D81" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>80</v>
-      </c>
-      <c r="B81">
-        <v>3</v>
-      </c>
-      <c r="C81" t="s">
+      <c r="E81" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="F81" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="F81" s="1" t="s">
+      <c r="G81" t="s">
+        <v>528</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>79</v>
+      </c>
+      <c r="B82">
+        <v>3</v>
+      </c>
+      <c r="D82" t="s">
         <v>191</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>80</v>
-      </c>
-      <c r="B82">
-        <v>3</v>
-      </c>
-      <c r="C82" t="s">
+      <c r="E82" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="F82" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="F82" s="1" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G82" t="s">
+        <v>529</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>395</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B83">
         <v>2</v>
       </c>
       <c r="D83" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
-    </row>
-    <row r="84" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G83" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B84">
         <v>3</v>
       </c>
-      <c r="C84" t="s">
+      <c r="D84" t="s">
+        <v>195</v>
+      </c>
+      <c r="E84" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="F84" s="1"/>
+      <c r="G84" t="s">
+        <v>530</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>79</v>
+      </c>
+      <c r="B85">
+        <v>3</v>
+      </c>
+      <c r="D85" t="s">
         <v>197</v>
       </c>
-      <c r="F84" s="1"/>
-    </row>
-    <row r="85" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>80</v>
-      </c>
-      <c r="B85">
-        <v>3</v>
-      </c>
-      <c r="C85" t="s">
+      <c r="E85" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="F85" s="1"/>
+      <c r="G85" t="s">
+        <v>531</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>79</v>
+      </c>
+      <c r="B86">
+        <v>3</v>
+      </c>
+      <c r="D86" t="s">
         <v>199</v>
       </c>
-      <c r="F85" s="1"/>
-    </row>
-    <row r="86" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>80</v>
-      </c>
-      <c r="B86">
-        <v>3</v>
-      </c>
-      <c r="C86" t="s">
+      <c r="E86" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="E86" s="1" t="s">
+      <c r="F86" s="1"/>
+      <c r="G86" t="s">
+        <v>532</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>79</v>
+      </c>
+      <c r="B87">
+        <v>3</v>
+      </c>
+      <c r="D87" t="s">
         <v>201</v>
       </c>
-      <c r="F86" s="1"/>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>80</v>
-      </c>
-      <c r="B87">
-        <v>3</v>
-      </c>
-      <c r="C87" t="s">
+      <c r="E87" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="E87" s="1" t="s">
+      <c r="F87" s="1"/>
+      <c r="G87" t="s">
+        <v>533</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>79</v>
+      </c>
+      <c r="B88">
+        <v>3</v>
+      </c>
+      <c r="D88" t="s">
         <v>203</v>
       </c>
-      <c r="F87" s="1"/>
-    </row>
-    <row r="88" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>80</v>
-      </c>
-      <c r="B88">
-        <v>3</v>
-      </c>
-      <c r="C88" t="s">
+      <c r="E88" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="E88" s="1" t="s">
+      <c r="F88" s="1"/>
+      <c r="G88" t="s">
+        <v>534</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>79</v>
+      </c>
+      <c r="B89">
+        <v>3</v>
+      </c>
+      <c r="D89" t="s">
         <v>205</v>
       </c>
-      <c r="F88" s="1"/>
-    </row>
-    <row r="89" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>80</v>
-      </c>
-      <c r="B89">
-        <v>3</v>
-      </c>
-      <c r="C89" t="s">
+      <c r="E89" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E89" s="1" t="s">
+      <c r="F89" s="1"/>
+      <c r="G89" t="s">
+        <v>535</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>79</v>
+      </c>
+      <c r="B90">
+        <v>3</v>
+      </c>
+      <c r="D90" t="s">
         <v>207</v>
       </c>
-      <c r="F89" s="1"/>
-    </row>
-    <row r="90" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>80</v>
-      </c>
-      <c r="B90">
-        <v>3</v>
-      </c>
-      <c r="C90" t="s">
+      <c r="E90" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="E90" s="1" t="s">
+      <c r="F90" s="1"/>
+      <c r="G90" t="s">
+        <v>536</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>79</v>
+      </c>
+      <c r="B91">
+        <v>3</v>
+      </c>
+      <c r="D91" t="s">
         <v>209</v>
       </c>
-      <c r="F90" s="1"/>
-    </row>
-    <row r="91" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A91" t="s">
-        <v>80</v>
-      </c>
-      <c r="B91">
-        <v>3</v>
-      </c>
-      <c r="C91" t="s">
+      <c r="E91" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="E91" s="1" t="s">
+      <c r="F91" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="F91" s="1" t="s">
+      <c r="G91" t="s">
+        <v>537</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>79</v>
+      </c>
+      <c r="B92">
+        <v>3</v>
+      </c>
+      <c r="D92" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A92" t="s">
-        <v>80</v>
-      </c>
-      <c r="B92">
-        <v>3</v>
-      </c>
-      <c r="C92" t="s">
+      <c r="E92" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="F92" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F92" s="1" t="s">
+      <c r="G92" t="s">
+        <v>538</v>
+      </c>
+      <c r="H92" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="I92" s="1" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>79</v>
+      </c>
+      <c r="B93">
+        <v>3</v>
+      </c>
+      <c r="D93" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A93" t="s">
-        <v>80</v>
-      </c>
-      <c r="B93">
-        <v>3</v>
-      </c>
-      <c r="C93" t="s">
+      <c r="E93" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E93" s="1" t="s">
+      <c r="F93" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F93" s="1" t="s">
+      <c r="G93" t="s">
+        <v>539</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>79</v>
+      </c>
+      <c r="B94">
+        <v>3</v>
+      </c>
+      <c r="D94" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A94" t="s">
-        <v>80</v>
-      </c>
-      <c r="B94">
-        <v>3</v>
-      </c>
-      <c r="C94" t="s">
+      <c r="E94" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E94" s="1" t="s">
+      <c r="F94" s="1"/>
+      <c r="G94" t="s">
+        <v>540</v>
+      </c>
+      <c r="H94" s="1" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>79</v>
+      </c>
+      <c r="B95">
+        <v>3</v>
+      </c>
+      <c r="D95" t="s">
         <v>220</v>
       </c>
-      <c r="F94" s="1"/>
-    </row>
-    <row r="95" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A95" t="s">
-        <v>80</v>
-      </c>
-      <c r="B95">
-        <v>3</v>
-      </c>
-      <c r="C95" t="s">
+      <c r="E95" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="E95" s="1" t="s">
+      <c r="F95" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="F95" s="1" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G95" t="s">
+        <v>541</v>
+      </c>
+      <c r="H95" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="I95" s="1" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B96">
         <v>2</v>
       </c>
       <c r="D96" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
-    </row>
-    <row r="97" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G96" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B97">
         <v>3</v>
       </c>
-      <c r="C97" t="s">
+      <c r="D97" t="s">
+        <v>224</v>
+      </c>
+      <c r="E97" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="E97" s="1" t="s">
+      <c r="F97" s="1"/>
+      <c r="G97" t="s">
+        <v>542</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>79</v>
+      </c>
+      <c r="B98">
+        <v>3</v>
+      </c>
+      <c r="D98" t="s">
         <v>226</v>
       </c>
-      <c r="F97" s="1"/>
-    </row>
-    <row r="98" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A98" t="s">
-        <v>80</v>
-      </c>
-      <c r="B98">
-        <v>3</v>
-      </c>
-      <c r="C98" t="s">
+      <c r="E98" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E98" s="1" t="s">
+      <c r="F98" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="F98" s="1" t="s">
+      <c r="G98" t="s">
+        <v>543</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>79</v>
+      </c>
+      <c r="B99">
+        <v>3</v>
+      </c>
+      <c r="D99" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A99" t="s">
-        <v>80</v>
-      </c>
-      <c r="B99">
-        <v>3</v>
-      </c>
-      <c r="C99" t="s">
+      <c r="E99" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E99" s="1" t="s">
+      <c r="F99" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="F99" s="1" t="s">
+      <c r="G99" t="s">
+        <v>544</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="I99" s="1" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>79</v>
+      </c>
+      <c r="B100">
+        <v>3</v>
+      </c>
+      <c r="D100" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A100" t="s">
-        <v>80</v>
-      </c>
-      <c r="B100">
-        <v>3</v>
-      </c>
-      <c r="C100" t="s">
+      <c r="E100" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="E100" s="1" t="s">
+      <c r="F100" s="1"/>
+      <c r="G100" t="s">
+        <v>545</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>79</v>
+      </c>
+      <c r="B101">
+        <v>3</v>
+      </c>
+      <c r="D101" t="s">
         <v>234</v>
       </c>
-      <c r="F100" s="1"/>
-    </row>
-    <row r="101" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A101" t="s">
-        <v>80</v>
-      </c>
-      <c r="B101">
-        <v>3</v>
-      </c>
-      <c r="C101" t="s">
+      <c r="E101" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="E101" s="1" t="s">
+      <c r="F101" s="1"/>
+      <c r="G101" t="s">
+        <v>546</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>79</v>
+      </c>
+      <c r="B102">
+        <v>3</v>
+      </c>
+      <c r="D102" t="s">
         <v>236</v>
       </c>
-      <c r="F101" s="1"/>
-    </row>
-    <row r="102" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A102" t="s">
-        <v>80</v>
-      </c>
-      <c r="B102">
-        <v>3</v>
-      </c>
-      <c r="C102" t="s">
+      <c r="E102" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="E102" s="1" t="s">
+      <c r="F102" s="1"/>
+      <c r="G102" t="s">
+        <v>547</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>79</v>
+      </c>
+      <c r="B103">
+        <v>3</v>
+      </c>
+      <c r="D103" t="s">
         <v>238</v>
       </c>
-      <c r="F102" s="1"/>
-    </row>
-    <row r="103" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A103" t="s">
-        <v>80</v>
-      </c>
-      <c r="B103">
-        <v>3</v>
-      </c>
-      <c r="C103" t="s">
+      <c r="E103" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="E103" s="1" t="s">
+      <c r="F103" s="1"/>
+      <c r="G103" t="s">
+        <v>548</v>
+      </c>
+      <c r="H103" s="1" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>79</v>
+      </c>
+      <c r="B104">
+        <v>3</v>
+      </c>
+      <c r="D104" t="s">
         <v>240</v>
       </c>
-      <c r="F103" s="1"/>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A104" t="s">
-        <v>80</v>
-      </c>
-      <c r="B104">
-        <v>3</v>
-      </c>
-      <c r="C104" t="s">
+      <c r="E104" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="E104" s="1" t="s">
+      <c r="F104" s="1"/>
+      <c r="G104" t="s">
+        <v>549</v>
+      </c>
+      <c r="H104" s="1" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>79</v>
+      </c>
+      <c r="B105">
+        <v>3</v>
+      </c>
+      <c r="D105" t="s">
         <v>242</v>
       </c>
-      <c r="F104" s="1"/>
-    </row>
-    <row r="105" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A105" t="s">
-        <v>80</v>
-      </c>
-      <c r="B105">
-        <v>3</v>
-      </c>
-      <c r="C105" t="s">
+      <c r="E105" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="E105" s="1" t="s">
+      <c r="F105" s="1"/>
+      <c r="G105" t="s">
+        <v>550</v>
+      </c>
+      <c r="H105" s="1" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>79</v>
+      </c>
+      <c r="B106">
+        <v>3</v>
+      </c>
+      <c r="D106" t="s">
         <v>244</v>
       </c>
-      <c r="F105" s="1"/>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A106" t="s">
-        <v>80</v>
-      </c>
-      <c r="B106">
-        <v>3</v>
-      </c>
-      <c r="C106" t="s">
+      <c r="E106" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="E106" s="1" t="s">
+      <c r="F106" s="1"/>
+      <c r="G106" t="s">
+        <v>551</v>
+      </c>
+      <c r="H106" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>79</v>
+      </c>
+      <c r="B107">
+        <v>3</v>
+      </c>
+      <c r="D107" t="s">
         <v>246</v>
       </c>
-      <c r="F106" s="1"/>
-    </row>
-    <row r="107" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A107" t="s">
-        <v>80</v>
-      </c>
-      <c r="B107">
-        <v>3</v>
-      </c>
-      <c r="C107" t="s">
+      <c r="E107" s="1" t="s">
         <v>247</v>
       </c>
-      <c r="E107" s="1" t="s">
+      <c r="F107" s="1"/>
+      <c r="G107" t="s">
+        <v>552</v>
+      </c>
+      <c r="H107" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>79</v>
+      </c>
+      <c r="B108">
+        <v>3</v>
+      </c>
+      <c r="D108" t="s">
         <v>248</v>
       </c>
-      <c r="F107" s="1"/>
-    </row>
-    <row r="108" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A108" t="s">
-        <v>80</v>
-      </c>
-      <c r="B108">
-        <v>3</v>
-      </c>
-      <c r="C108" t="s">
+      <c r="E108" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="E108" s="1" t="s">
+      <c r="F108" s="1"/>
+      <c r="G108" t="s">
+        <v>553</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>79</v>
+      </c>
+      <c r="B109">
+        <v>3</v>
+      </c>
+      <c r="D109" t="s">
         <v>250</v>
       </c>
-      <c r="F108" s="1"/>
-    </row>
-    <row r="109" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A109" t="s">
-        <v>80</v>
-      </c>
-      <c r="B109">
-        <v>3</v>
-      </c>
-      <c r="C109" t="s">
+      <c r="E109" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E109" s="1" t="s">
+      <c r="F109" s="1"/>
+      <c r="G109" t="s">
+        <v>554</v>
+      </c>
+      <c r="H109" s="1" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>79</v>
+      </c>
+      <c r="B110">
+        <v>3</v>
+      </c>
+      <c r="D110" t="s">
         <v>252</v>
       </c>
-      <c r="F109" s="1"/>
-    </row>
-    <row r="110" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A110" t="s">
-        <v>80</v>
-      </c>
-      <c r="B110">
-        <v>3</v>
-      </c>
-      <c r="C110" t="s">
+      <c r="E110" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="E110" s="1" t="s">
-        <v>254</v>
-      </c>
       <c r="F110" s="1"/>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G110" t="s">
+        <v>555</v>
+      </c>
+      <c r="H110" s="1" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B111">
         <v>2</v>
       </c>
       <c r="D111" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
-    </row>
-    <row r="112" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G111" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B112">
         <v>3</v>
       </c>
-      <c r="C112" t="s">
+      <c r="D112" t="s">
+        <v>255</v>
+      </c>
+      <c r="E112" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="E112" s="1" t="s">
+      <c r="F112" s="1"/>
+      <c r="G112" t="s">
+        <v>556</v>
+      </c>
+      <c r="H112" s="1" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>79</v>
+      </c>
+      <c r="B113">
+        <v>3</v>
+      </c>
+      <c r="D113" t="s">
         <v>257</v>
       </c>
-      <c r="F112" s="1"/>
-    </row>
-    <row r="113" spans="1:6" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A113" t="s">
-        <v>80</v>
-      </c>
-      <c r="B113">
-        <v>3</v>
-      </c>
-      <c r="C113" t="s">
+      <c r="E113" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="E113" s="1" t="s">
+      <c r="F113" s="1"/>
+      <c r="G113" t="s">
+        <v>557</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>79</v>
+      </c>
+      <c r="B114">
+        <v>3</v>
+      </c>
+      <c r="D114" t="s">
         <v>259</v>
       </c>
-      <c r="F113" s="1"/>
-    </row>
-    <row r="114" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A114" t="s">
-        <v>80</v>
-      </c>
-      <c r="B114">
-        <v>3</v>
-      </c>
-      <c r="C114" t="s">
+      <c r="E114" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="E114" s="1" t="s">
+      <c r="F114" s="1"/>
+      <c r="G114" t="s">
+        <v>558</v>
+      </c>
+      <c r="H114" s="1" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>79</v>
+      </c>
+      <c r="B115">
+        <v>3</v>
+      </c>
+      <c r="D115" t="s">
         <v>261</v>
       </c>
-      <c r="F114" s="1"/>
-    </row>
-    <row r="115" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A115" t="s">
-        <v>80</v>
-      </c>
-      <c r="B115">
-        <v>3</v>
-      </c>
-      <c r="C115" t="s">
+      <c r="E115" s="1" t="s">
         <v>262</v>
       </c>
-      <c r="E115" s="1" t="s">
-        <v>263</v>
-      </c>
       <c r="F115" s="1"/>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G115" t="s">
+        <v>559</v>
+      </c>
+      <c r="H115" s="1" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B116">
         <v>1</v>
       </c>
       <c r="D116" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
-    </row>
-    <row r="117" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G116" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B117">
         <v>2</v>
       </c>
-      <c r="C117" t="s">
+      <c r="D117" t="s">
+        <v>264</v>
+      </c>
+      <c r="E117" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="E117" s="1" t="s">
-        <v>266</v>
-      </c>
       <c r="F117" s="1"/>
-    </row>
-    <row r="118" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="G117" t="s">
+        <v>560</v>
+      </c>
+      <c r="H117" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B118">
         <v>2</v>
       </c>
-      <c r="C118" t="s">
+      <c r="D118" t="s">
+        <v>266</v>
+      </c>
+      <c r="E118" s="1" t="s">
         <v>267</v>
       </c>
-      <c r="E118" s="1" t="s">
+      <c r="F118" s="1" t="s">
         <v>268</v>
       </c>
-      <c r="F118" s="1" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G118" t="s">
+        <v>561</v>
+      </c>
+      <c r="H118" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="I118" s="1" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B119">
         <v>2</v>
       </c>
-      <c r="C119" t="s">
+      <c r="D119" t="s">
+        <v>269</v>
+      </c>
+      <c r="E119" s="1" t="s">
         <v>270</v>
       </c>
-      <c r="E119" s="1" t="s">
-        <v>271</v>
-      </c>
       <c r="F119" s="1"/>
-    </row>
-    <row r="120" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="G119" t="s">
+        <v>562</v>
+      </c>
+      <c r="H119" s="1" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B120">
         <v>2</v>
       </c>
-      <c r="C120" t="s">
+      <c r="D120" t="s">
+        <v>271</v>
+      </c>
+      <c r="E120" s="1" t="s">
         <v>272</v>
       </c>
-      <c r="E120" s="1" t="s">
-        <v>273</v>
-      </c>
       <c r="F120" s="1"/>
-    </row>
-    <row r="121" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G120" t="s">
+        <v>563</v>
+      </c>
+      <c r="H120" s="1" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B121">
         <v>2</v>
       </c>
-      <c r="C121" t="s">
+      <c r="D121" t="s">
+        <v>273</v>
+      </c>
+      <c r="E121" s="1" t="s">
         <v>274</v>
       </c>
-      <c r="E121" s="1" t="s">
-        <v>275</v>
-      </c>
       <c r="F121" s="1"/>
-    </row>
-    <row r="122" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G121" t="s">
+        <v>564</v>
+      </c>
+      <c r="H121" s="1" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B122">
         <v>2</v>
       </c>
-      <c r="C122" t="s">
+      <c r="D122" t="s">
+        <v>275</v>
+      </c>
+      <c r="E122" s="1" t="s">
         <v>276</v>
       </c>
-      <c r="E122" s="1" t="s">
-        <v>277</v>
-      </c>
       <c r="F122" s="1"/>
-    </row>
-    <row r="123" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G122" t="s">
+        <v>565</v>
+      </c>
+      <c r="H122" s="1" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B123">
         <v>2</v>
       </c>
-      <c r="C123" t="s">
+      <c r="D123" t="s">
+        <v>277</v>
+      </c>
+      <c r="E123" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="E123" s="1" t="s">
+      <c r="F123" s="1" t="s">
         <v>279</v>
       </c>
-      <c r="F123" s="1" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G123" t="s">
+        <v>566</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B124">
         <v>2</v>
       </c>
-      <c r="C124" t="s">
+      <c r="D124" t="s">
+        <v>280</v>
+      </c>
+      <c r="E124" s="1" t="s">
         <v>281</v>
       </c>
-      <c r="E124" s="1" t="s">
-        <v>282</v>
-      </c>
       <c r="F124" s="1"/>
-    </row>
-    <row r="125" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G124" t="s">
+        <v>567</v>
+      </c>
+      <c r="H124" s="1" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B125">
         <v>2</v>
       </c>
-      <c r="C125" t="s">
+      <c r="D125" t="s">
+        <v>282</v>
+      </c>
+      <c r="E125" s="1" t="s">
         <v>283</v>
       </c>
-      <c r="E125" s="1" t="s">
-        <v>284</v>
-      </c>
       <c r="F125" s="1"/>
-    </row>
-    <row r="126" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="G125" t="s">
+        <v>568</v>
+      </c>
+      <c r="H125" s="1" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" ht="72" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B126">
         <v>2</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D126" t="s">
+        <v>284</v>
+      </c>
+      <c r="E126" s="1" t="s">
         <v>285</v>
       </c>
-      <c r="E126" s="1" t="s">
+      <c r="F126" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="F126" s="1" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="G126" t="s">
+        <v>569</v>
+      </c>
+      <c r="H126" s="1" t="s">
+        <v>447</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B127">
         <v>2</v>
       </c>
-      <c r="C127" t="s">
+      <c r="D127" t="s">
+        <v>287</v>
+      </c>
+      <c r="E127" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="E127" s="1" t="s">
-        <v>289</v>
-      </c>
       <c r="F127" s="1"/>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G127" t="s">
+        <v>570</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B128">
         <v>1</v>
       </c>
       <c r="D128" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
-    </row>
-    <row r="129" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="G128" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B129">
         <v>2</v>
       </c>
-      <c r="C129" t="s">
+      <c r="D129" t="s">
+        <v>290</v>
+      </c>
+      <c r="E129" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="E129" s="1" t="s">
-        <v>292</v>
-      </c>
       <c r="F129" s="1"/>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G129" t="s">
+        <v>571</v>
+      </c>
+      <c r="H129" s="1" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B130">
         <v>1</v>
       </c>
       <c r="D130" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G130" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B131">
         <v>2</v>
       </c>
       <c r="D131" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
-    </row>
-    <row r="132" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+      <c r="G131" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="132" spans="1:8" ht="72" x14ac:dyDescent="0.3">
       <c r="B132">
         <v>3</v>
       </c>
-      <c r="C132" t="s">
+      <c r="D132" t="s">
+        <v>294</v>
+      </c>
+      <c r="E132" s="1" t="s">
         <v>295</v>
       </c>
-      <c r="E132" s="1" t="s">
-        <v>296</v>
-      </c>
       <c r="F132" s="1"/>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="G132" s="3" t="s">
+        <v>572</v>
+      </c>
+      <c r="H132" s="1" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B133">
         <v>2</v>
       </c>
       <c r="D133" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
-    </row>
-    <row r="134" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="G133" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="134" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B134">
         <v>3</v>
       </c>
-      <c r="C134" t="s">
+      <c r="D134" t="s">
+        <v>297</v>
+      </c>
+      <c r="E134" s="1" t="s">
         <v>298</v>
       </c>
-      <c r="E134" s="1" t="s">
-        <v>299</v>
-      </c>
       <c r="F134" s="1"/>
+      <c r="G134" s="4" t="s">
+        <v>573</v>
+      </c>
+      <c r="H134" s="1" t="s">
+        <v>456</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add Italian Version + Assessability Fix
The Excel and YAML files contain English, French and Italian versions.
</commit_message>
<xml_diff>
--- a/tools/excel/finma/finma-2023-01.xlsx
+++ b/tools/excel/finma/finma-2023-01.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\finma\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBBC348B-A444-42DF-836B-BD9EA0B01118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{089F2018-1982-4005-9FEA-F8BEB3233BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="574">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="848">
   <si>
     <t>type</t>
   </si>
@@ -1772,6 +1772,841 @@
   </si>
   <si>
     <t>Margin no. 114</t>
+  </si>
+  <si>
+    <t>name[it]</t>
+  </si>
+  <si>
+    <t>description[it]</t>
+  </si>
+  <si>
+    <t>annotation[it]</t>
+  </si>
+  <si>
+    <t>I. Oggetto e campo di applicazione</t>
+  </si>
+  <si>
+    <t>nm. 1</t>
+  </si>
+  <si>
+    <t>La presente circolare si riferisce alle prescrizioni dell’Ordinanza sulle banche (artt. 12 e 14e OBCR; RS 952.02) e dell’Ordinanza sugli istituti finanziari (artt. 12 e 68 OIsFi; RS 954.11) concernenti la separazione delle funzioni, la gestione dei rischi e il controllo interno e concretizza la prassi di vigilanza in materia. Tiene conto dei Principi del Comitato di Basilea sulla sana gestione dei rischi operativi1 e sulla resilienza operativa2.</t>
+  </si>
+  <si>
+    <t>[1] BCBS Revisions to the Principles for the Sound Management of Operational Risk (31 marzo 2021).
+[2] BCBS Principles for Operational Resilience (31 marzo 2021).</t>
+  </si>
+  <si>
+    <t>nm. 2</t>
+  </si>
+  <si>
+    <t>La circolare è destinata alle banche secondo l’art. 1a e alle persone secondo l’art. 1b della Legge sulle banche (LBCR; RS 952.0), alle società di intermediazione mobiliare secondo l’art. 2 cpv. 1 lett. e e l’art. 41 della Legge sugli istituti finanziari (LIsFI; RS 954.1) nonché ai gruppi finanziari e ai conglomerati finanziari secondo l’art. 3c LBCR e l’art. 49 LIsFi. Di seguito le banche, le persone secondo l’art. 1b LBCR, le società di intermediazione mobiliare, i gruppi finanziari e i conglomerati finanziari vengono denominati congiuntamente «istituti».</t>
+  </si>
+  <si>
+    <t>II. Definizioni</t>
+  </si>
+  <si>
+    <t>nm. 3</t>
+  </si>
+  <si>
+    <t>I rischi operativi sono definiti nell’art. 89 dell’Ordinanza sui fondi propri (OFoP; RS 952.03). Consistono nel pericolo di incorrere in perdite finanziarie dovute all’inadeguatezza o all’inefficacia delle procedure o dei sistemi interni, all’inadeguatezza delle azioni delle persone o a errori da esse commessi oppure causate da eventi esterni. Essi comprendono le perdite finanziarie che possono insorgere da rischi legali o di compliance. La gestione dei rischi operativi tiene tipicamente conto anche di altre dimensioni del danno3, nella misura in cui esse possano causare tra l’altro perdite finanziarie. Sono esclusi i rischi strategici.</t>
+  </si>
+  <si>
+    <t>[3] Per esempio effetti negativi sulla reputazione, possibile perdita di fiducia e di clienti, effetti negativi sul mercato, effetti regolatori negativi (p. es. possibile perdita della licenza).</t>
+  </si>
+  <si>
+    <t>nm. 4</t>
+  </si>
+  <si>
+    <t>I rischi inerenti sono rischi operativi a cui l’istituto è esposto a causa dei suoi prodotti, processi e sistemi e delle sue attività senza considerare le misure di controllo e di attenuazione.</t>
+  </si>
+  <si>
+    <t>nm. 5</t>
+  </si>
+  <si>
+    <t>I rischi residui sono rischi operativi a cui l’istituto è esposto dopo aver considerato le misure di controllo e di attenuazione.</t>
+  </si>
+  <si>
+    <t>nm. 6</t>
+  </si>
+  <si>
+    <t>Le tecnologie dell'informazione e della comunicazione (TIC) designano la struttura fisica e logica (elettronica) dei sistemi informatici e di comunicazione, le singoli componenti hardware e software, le reti, i dati e gli ambienti operativi.</t>
+  </si>
+  <si>
+    <t>nm. 7</t>
+  </si>
+  <si>
+    <t>I dati critici sono dati che, in considerazione delle dimensioni, della complessità, della struttura, del profilo di rischio e del modello commerciale dell’istituto sono importanti a tal punto da richiedere uno standard più elevato di sicurezza. Si tratta di dati essenziali ai fini dell’erogazione efficace e continuativa dei servizi dell’istituto o per scopi regolatori. Per valutare e determinare la criticità dei dati è necessario considerarne sia la confidenzialità sia l’integrità e la disponibilità. Ognuno di questi tre aspetti può essere determinante per classificare i dati come critici.</t>
+  </si>
+  <si>
+    <t>nm. 8</t>
+  </si>
+  <si>
+    <t>I processi critici sono processi la cui perturbazione importante o interruzione compromette lo svolgimento delle funzioni critiche, di cui sono parte.</t>
+  </si>
+  <si>
+    <t>nm. 9</t>
+  </si>
+  <si>
+    <t>Il business continuity management (BCM) designa l’approccio adottato a livello di istituto per ripristinare i processi critici in caso di perturbazione o interruzione importante che vada al di là della gestione degli incidenti. Definisce dunque la reazione a perturbazioni importanti o interruzioni. Un BCM efficace riduce i rischi residui correlati a perturbazioni importanti o interruzioni.</t>
+  </si>
+  <si>
+    <t>nm. 10</t>
+  </si>
+  <si>
+    <t>Il recovery time objective (RTO) è il tempo necessario per ripristinare un’applicazione, un sistema e/o un processo. Il recovery point objective (RPO) è la durata massima tollerabile di una perdita di dati.</t>
+  </si>
+  <si>
+    <t>nm. 11</t>
+  </si>
+  <si>
+    <t>Il business continuity plan (BCP) è un piano previdente che definisce le procedure, le opzioni di ripristino e le risorse sostitutive necessarie (i processi di ripristino) per garantire la continuità e il ripristino dei processi critici.</t>
+  </si>
+  <si>
+    <t>nm. 12</t>
+  </si>
+  <si>
+    <t>Il disaster recovery plan (DRP) definisce i processi di ripristino necessari per conseguire gli obiettivi di ripristino in caso di un guasto grave o di distruzione delle tecnologie dell’informazione e della comunicazione (TIC) e in considerazione dell’eventuale assenza di persone chiave.</t>
+  </si>
+  <si>
+    <t>nm. 13</t>
+  </si>
+  <si>
+    <t>Le situazioni di crisi sono situazioni straordinarie, che costituiscono una potenziale minaccia per l’esistenza e non possono essere fronteggiate con misure e competenze decisionali ordinarie. Si distinguono dagli incidenti (incidents) e dalle perturbazioni o dalle interruzioni importanti che possono essere fronteggiate con la gestione degli incidenti nell’esercizio normale o con i BCP e i DRP stabiliti.</t>
+  </si>
+  <si>
+    <t>nm. 14</t>
+  </si>
+  <si>
+    <t>Le funzioni critiche comprendono:</t>
+  </si>
+  <si>
+    <t>nm. 15</t>
+  </si>
+  <si>
+    <t>a. le attività, i processi e i servizi, incluse le risorse sottostanti necessarie al loro svolgimento, la cui interruzione pregiudicherebbe il mantenimento dell’attività dell’istituto o il suo ruolo sul mercato finanziario, quindi anche la funzionalità dei mercati finanziari; e</t>
+  </si>
+  <si>
+    <t>nm. 16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b. le funzioni di rilevanza sistemica secondo l’art. 8 LBCR. </t>
+  </si>
+  <si>
+    <t>nm. 17</t>
+  </si>
+  <si>
+    <t>La tolleranza alle interruzioni è la portata (p. es. durata o danni attesi) dell’interruzione di una funzione critica, che l’istituto è disposto ad accettare considerando scenari gravi, ma plausibili. Per ogni funzione critica deve essere definita una tolleranza alle interruzioni.</t>
+  </si>
+  <si>
+    <t>nm. 18</t>
+  </si>
+  <si>
+    <t>La resilienza operativa designa la capacità dell’istituto di ripristinare le sue funzioni critiche in caso di interruzioni entro i limiti di tolleranza alle interruzioni, ossia la capacità dell’istituto di individuare minacce e possibili disfunzioni, proteggersi da esse e reagire, ripristinare l’attività ordinaria in caso di interruzioni e trarne insegnamenti per minimizzare le conseguenze sullo svolgimento delle funzioni critiche. Un istituto operativamente resiliente ha strutturato il suo modello operativo4 in modo tale da essere meno esposto al rischio di interruzioni in riferimento alle sue funzioni critiche. La resilienza operativa riduce quindi non solo i rischi residui delle interruzioni, ma anche il rischio inerente che si verifichino interruzioni. Una gestione efficace dei rischi operativi contribuisce a rafforzare la resilienza operativa dell’istituto.</t>
+  </si>
+  <si>
+    <t>[4] Spesso chiamato anche resilience by design.</t>
+  </si>
+  <si>
+    <t>III. Principio di proporzionalità</t>
+  </si>
+  <si>
+    <t>nm. 19</t>
+  </si>
+  <si>
+    <t>La presente circolare si applica fondamentalmente a tutti i suoi destinatari, tuttavia i requisiti da adempiere nel singolo caso si differenziano in funzione delle dimensioni, della complessità, della struttura e del profilo di rischio dell’istituto. Nel singolo caso, la FINMA può ordinare facilitazioni o inasprimenti.</t>
+  </si>
+  <si>
+    <t>nm. 20</t>
+  </si>
+  <si>
+    <t>Le banche e le società di intermediazione mobiliare delle categorie FINMA 4 e 5 sono esentate dall’adempimento dei numeri marginali 33–38, 41–46, 48, 51, 57, 73, 74, 76–78, 80, 87, 92, 93, 96, 103, 104 e 110–112.</t>
+  </si>
+  <si>
+    <t>nm. 21</t>
+  </si>
+  <si>
+    <t>Gli istituti di cui agli artt. 47a–47e OFoP, le persone secondo l’art. 1b LBCR e le società di intermediazione mobiliare che non tengono conti sono inoltre esentate dall’adempimento dei numeri marginali 72, 75, 79 e 105–109.</t>
+  </si>
+  <si>
+    <t>IV. Gestione dei rischi operativi</t>
+  </si>
+  <si>
+    <t>A. Gestione trasversale dei rischi operativi</t>
+  </si>
+  <si>
+    <t>nm. 22</t>
+  </si>
+  <si>
+    <t>La gestione dei rischi operativi rientra nella gestione del rischio a livello di istituto conformemente alla Circolare FINMA 17/1 «Corporate governance – banche».</t>
+  </si>
+  <si>
+    <t>nm. 23</t>
+  </si>
+  <si>
+    <t>L’organo preposto all’alta direzione approva i principi della gestione dei rischi operativi rilevanti per l’istituto e vigila sulla loro osservanza. Vi rientrano, tra l’altro, i rischi TIC, i cyber-rischi, i rischi concernenti i dati critici, i rischi derivanti dalla configurazione e dell’implementazione del BCM ed eventualmente i rischi afferenti alle prestazioni di servizio transfrontaliere. Almeno una volta all’anno approva la tolleranza al rischio per i rischi operativi conformemente alla politica di rischio in considerazione degli obiettivi strategici e finanziari dell’istituto. Al riguardo considera i risultati delle valutazioni del rischio e dei controlli secondo il nm. 30. Accetta la misura dell’esposizione ai rischi operativi da parte dell’istituto oppure decide un adeguamento della tolleranza al rischio e i necessari cambiamenti a livello strategico5.</t>
+  </si>
+  <si>
+    <t>[5] Per esempio un cambiamento del modello commerciale.</t>
+  </si>
+  <si>
+    <t>nm. 24</t>
+  </si>
+  <si>
+    <t>L’organo preposto all’alta direzione approva periodicamente le strategie di gestione delle TIC, dei cyber-rischi, dei dati critici e del BCM e vigila sulla loro osservanza.</t>
+  </si>
+  <si>
+    <t>nm. 25</t>
+  </si>
+  <si>
+    <t>La direzione assicura in modo attendibile che i rischi operativi siano identificati, valutati, limitati e monitorati e che l’efficacia sia della configurazione sia dell’attuazione di tale gestione dei rischi operativi sia periodicamente verificata. Per limitare i rischi inerenti considerati essenziali6 adotta misure integrative o inasprimenti in funzione del rischio specifico.</t>
+  </si>
+  <si>
+    <t>[6] Spesso chiamati rischi chiave (key risks).</t>
+  </si>
+  <si>
+    <t>nm. 26</t>
+  </si>
+  <si>
+    <t>Per rendere i collaboratori sempre più consapevoli dell’importanza di ridurre i rischi operativi rilevanti, in particolare i rischi TIC, i cyber-rischi, i rischi concernenti i dati critici e i rischi derivanti dalla configurazione e dall’implementazione del BCM, è necessario implementare misure tenendo in considerazione i loro compiti, le competenze e le responsabilità (CCR)7.</t>
+  </si>
+  <si>
+    <t>[7] Ciò implica, tra l’altro, la selezione accurata e la qualificazione del personale per i CCR e la formazione continua nel quadro delle sue attività.</t>
+  </si>
+  <si>
+    <t>nm. 27</t>
+  </si>
+  <si>
+    <t>Se necessario, nell’ambito della vigilanza continua la FINMA definisce ulteriori requisiti in materia di gestione dei rischi operativi per temi specifici. Ciò avviene con moderazione e applicando il principio di proporzionalità.</t>
+  </si>
+  <si>
+    <t>nm. 28</t>
+  </si>
+  <si>
+    <t>I rischi operativi devono essere categorizzati secondo criteri unitari a livello di istituto e inventariati. Questa categorizzazione può essere effettuata rifacendosi alla categorizzazione utilizzata nel calcolo dei fondi propri minimi per i rischi operativi o mediante una tassonomia interna. Essa deve essere applicata in modo sistematico in tutti i settori dell’istituto e in tutte le componenti della gestione dei rischi operativi.</t>
+  </si>
+  <si>
+    <t>nm. 29</t>
+  </si>
+  <si>
+    <t>Per identificare i rischi operativi vengono considerati fattori interni8 ed esterni9. I rischi operativi individuati sono valutati in modo attendibile nell’ottica sia dei rischi inerenti sia di quelli residui.</t>
+  </si>
+  <si>
+    <t>[8] Sono considerati fattori interni, per esempio, i cambiamenti apportati ai prodotti, alle attività, ai processi e ai sistemi, i risultati dell’audit e le perdite interne derivanti dai rischi operativi.
+[9] Sono considerati fattori esterni, per esempio, gli eventi che generano perdite in altri istituti, i cambiamenti sul piano della sicurezza (p. es. dovuti a impatti ambientali, cyber-attacchi o terrorismo) o gli adeguamenti ai requisiti normativi.</t>
+  </si>
+  <si>
+    <t>nm. 30</t>
+  </si>
+  <si>
+    <t>L’identificazione e la valutazione dei rischi operativi si basano almeno sui risultati dell’audit10 e sulle valutazioni dei rischi e dei controlli da effettuare regolarmente. Tali valutazioni tengono conto dei rischi inerenti, dell’efficacia delle misure di controllo e di attenuazione esistenti e dei rischi residui.</t>
+  </si>
+  <si>
+    <t>[10] In questo caso i risultati dell’audit comprendono gli esiti della revisione interna e della società di audit esterna, se disponibili, nonché i risultati delle verifiche svolte, per esempio, dalle divisioni commerciali e organizzative, dal con- trollo del rischio, dalla funzione preposta alla compliance o dalle autorità di vigilanza.</t>
+  </si>
+  <si>
+    <t>nm. 31</t>
+  </si>
+  <si>
+    <t>Per valutare le misure di controllo e di attenuazione esistenti si procede in particolare a un esame regolare dell’efficacia dei controlli chiave da parte di un’istanza di controllo indipendente (design effectiveness e operating effectiveness testing), documentandone i risultati. I controlli chiave sono le misure di controllo e di attenuazione che minimizzano i rischi inerenti considerati essenziali. Anche la separazione dei CCR per garantire l’indipendenza e prevenire i conflitti di interessi è oggetto di valutazioni periodiche.</t>
+  </si>
+  <si>
+    <t>nm. 32</t>
+  </si>
+  <si>
+    <t>Prima di apportare cambiamenti sostanziali a livello di prodotti, attività, processi e sistemi è necessario effettuare valutazioni ad hoc dei rischi e dei controlli, che prendono in considerazione i rischi operativi derivanti dal processo di cambiamento e i rischi operativi delle condizioni target. Ove necessario, vengono adeguati i limiti di tolleranza al rischio e attuate misure di controllo e di attenuazione.</t>
+  </si>
+  <si>
+    <t>nm. 33</t>
+  </si>
+  <si>
+    <t>In funzione della natura, della portata, della complessità e del rischio dei prodotti, delle attività, dei processi e dei sistemi specifici all’istituto, devono essere applicati gli ulteriori strumenti e metodi seguenti:</t>
+  </si>
+  <si>
+    <t>nm. 34</t>
+  </si>
+  <si>
+    <t>a. raccolta e analisi sistematiche dei dati interni di perdita e degli eventi esterni rilevanti correlati a rischi operativi;</t>
+  </si>
+  <si>
+    <t>nm. 35</t>
+  </si>
+  <si>
+    <t>b. indicatori di rischio e di controllo per il monitoraggio dei rischi operativi e la tempestiva identificazione degli aumenti rilevanti dei rischi;</t>
+  </si>
+  <si>
+    <t>nm. 36</t>
+  </si>
+  <si>
+    <t>c. analisi di scenario e/o stima del potenziale di perdita in considerazione dei o rispetto ai fondi propri minimi per i rischi operativi;</t>
+  </si>
+  <si>
+    <t>nm. 37</t>
+  </si>
+  <si>
+    <t>d. analisi comparative (read-across), per esempio analisi della rilevanza dei risultati dell’audit in altri settori dell’istituto o confronti tra i risultati delle valutazioni del rischio e dei controlli di diversi settori.</t>
+  </si>
+  <si>
+    <t>nm. 38</t>
+  </si>
+  <si>
+    <t>La tolleranza al rischio per i rischi operativi tiene conto della tolleranza in rapporto ai rischi operativi inerenti11 e a quelli residui ed è monitorata mediante indicatori di rischio o di controllo.</t>
+  </si>
+  <si>
+    <t>[11] La tolleranza al rischio in riferimento ai rischi inerenti considera decisioni strategiche che concernono il modello com- merciale o operativo, per esempio la tolleranza per i rischi inerenti implicati dall’erogazione di servizi a determinati segmenti di clientela o Paesi, dall’offerta di determinati prodotti, dall’applicazione di processi prevalentemente ma- nuali, dall’utilizzo di un’infrastruttura informatica complessa o da determinate esternalizzazioni (outsourcing).</t>
+  </si>
+  <si>
+    <t>nm. 39</t>
+  </si>
+  <si>
+    <t>Il controllo dei rischi presenta all’organo preposto all’alta direzione almeno una volta all’anno e alla direzione almeno a ritmo semestrale in conformità ai nm. 75–76 della Circolare FINMA 17/1 un rapporto sui rischi operativi al massimo livello12 della categorizzazione definita secondo il nm. 28, sul loro confronto con la tolleranza al rischio stabilita e sui dettagli concernenti le perdite interne sostanziali.</t>
+  </si>
+  <si>
+    <t>[12] Il massimo livello della categorizzazione viene spesso chiamato livello 1 o level 1. Il rapporto può essere effettuato anche a un livello più dettagliato.</t>
+  </si>
+  <si>
+    <t>nm. 40</t>
+  </si>
+  <si>
+    <t>In riferimento ai rischi TIC e ai cyber-rischi rilevanti, il rapporto da presentare alla direzione almeno una volta all’anno contiene inoltre informazioni sull’evoluzione di tali rischi, sull’efficacia dei relativi controlli chiave e su importanti eventi interni ed esterni in relazione a tali rischi.</t>
+  </si>
+  <si>
+    <t>nm. 41</t>
+  </si>
+  <si>
+    <t>Il rapporto interno di cui al nm. 39 contiene a titolo complementare le seguenti informazioni:</t>
+  </si>
+  <si>
+    <t>nm. 42</t>
+  </si>
+  <si>
+    <t>• i fattori esterni rilevanti secondo la nota 9,</t>
+  </si>
+  <si>
+    <t>nm. 43</t>
+  </si>
+  <si>
+    <t>• una panoramica ricapitolativa sull’efficacia dei controlli chiave secondo il nm. 31,</t>
+  </si>
+  <si>
+    <t>nm. 44</t>
+  </si>
+  <si>
+    <t>• i rischi operativi emergenti,</t>
+  </si>
+  <si>
+    <t>nm. 45</t>
+  </si>
+  <si>
+    <t>• i risultati derivanti dall’applicazione degli ulteriori strumenti e metodi secondo il nm. 33.</t>
+  </si>
+  <si>
+    <t>nm. 46</t>
+  </si>
+  <si>
+    <t>Conformemente al principio di proporzionalità, per le banche di rilevanza sistemica viene presentato un resoconto periodico sui rischi operativi anche al livello delle divisioni commerciali e organizzative esposte a rischi operativi rilevanti o essenziali.</t>
+  </si>
+  <si>
+    <t>B. Gestione dei rischi TIC</t>
+  </si>
+  <si>
+    <t>a) Strategia TIC e governance</t>
+  </si>
+  <si>
+    <t>nm. 47</t>
+  </si>
+  <si>
+    <t>Le aspettative fondamentali poste alla strategia, alla governance e al rafforzamento della consapevolezza in riferimento alle TIC sono enunciate nei nm. 23–26 e 40.</t>
+  </si>
+  <si>
+    <t>nm. 48</t>
+  </si>
+  <si>
+    <t>La gestione dei rischi TIC considera standard e pratiche rilevanti riconosciuti a livello internazionale, nonché l’impatto di nuovi sviluppi tecnologici sui rischi TIC.</t>
+  </si>
+  <si>
+    <t>nm. 49</t>
+  </si>
+  <si>
+    <t>La direzione assicura, sia per la gestione del cambiamento (change management) sia per l’esercizio delle TIC (run, maintenance), l’implementazione e la documentazione di procedure, processi, controlli e CCR, a cui sono assegnate risorse qualificate e appropriate.</t>
+  </si>
+  <si>
+    <t>b) Gestione del cambiamento (change management)</t>
+  </si>
+  <si>
+    <t>nm. 50</t>
+  </si>
+  <si>
+    <t>La gestione del cambiamento definisce procedure, processi e controlli per tutte le fasi dello sviluppo o dell’acquisto di TIC e, in ognuna di queste fasi, considera l’impatto del cambiamento sui rischi TIC, focalizzandosi sui requisiti in materia di confidenzialità, integrità e disponibilità.</t>
+  </si>
+  <si>
+    <t>nm. 51</t>
+  </si>
+  <si>
+    <t>Occorre garantire una separazione tra gli ambienti di sviluppo o di test delle TIC e l’ambiente della loro produzione. Ciò comprende anche una chiara attribuzione dei CCR e la regolamentazione dei conseguenti diritti di accesso.</t>
+  </si>
+  <si>
+    <t>nm. 52</t>
+  </si>
+  <si>
+    <t>Nelle fasi di sviluppo e di acquisto delle TIC le esigenze funzionali e non funzionali13 sono definite chiaramente e approvate, quindi testate e convalidate in funzione della loro criticità.</t>
+  </si>
+  <si>
+    <t>[13] P. es. per quanto attiene all’architettura o ai requisiti di sicurezza delle informazioni.</t>
+  </si>
+  <si>
+    <t>c) Esercizio delle TIC (run, maintenance)</t>
+  </si>
+  <si>
+    <t>nm. 53</t>
+  </si>
+  <si>
+    <t>L’istituto tiene uno o più inventari delle componenti TIC. L’inventario include componenti hardware e software nonché i luoghi di archiviazione di dati critici. Tiene conto delle dipendenze all’interno dell’istituto e delle interfacce con importanti fornitori esterni di servizi.</t>
+  </si>
+  <si>
+    <t>nm. 54</t>
+  </si>
+  <si>
+    <t>L’inventario, disponibile in tempi brevi, viene regolarmente verificato in termini di completezza ed esattezza e aggiornato.</t>
+  </si>
+  <si>
+    <t>nm. 55</t>
+  </si>
+  <si>
+    <t>L’istituto dispone di procedure, processi e controlli che garantiscono la confidenzialità, l’integrità e la disponibilità dell’ambiente di produzione delle TIC considerando la rispettiva tolleranza al rischio.</t>
+  </si>
+  <si>
+    <t>nm. 56</t>
+  </si>
+  <si>
+    <t>L’istituto garantisce il passaggio senza difficoltà dall’esercizio delle TIC ai suoi processi BCP e DRP in caso di perturbazioni importanti o interruzioni. Implementa opportuni processi di backup e di ripristino, che sono regolarmente testati e convalidati.</t>
+  </si>
+  <si>
+    <t>nm. 57</t>
+  </si>
+  <si>
+    <t>L’istituto dispone di procedure, processi e controlli che garantiscono una gestione orientata al rischio delle TIC la cui vita operativa volge al termine o che hanno superato il periodo di disattivazione previsto.</t>
+  </si>
+  <si>
+    <t>d) Gestione degli incidenti (incident management)</t>
+  </si>
+  <si>
+    <t>nm. 58</t>
+  </si>
+  <si>
+    <t>L’istituto dispone di procedure, processi e controlli volti a trattare incidenti TIC rilevanti, inclusi quelli riconducibili a dipendenze da importanti fornitori esterni di servizi e da esternalizzazioni in seno al gruppo. Al riguardo è necessario considerare l’intero ciclo di vita degli incidenti TIC importanti e definire i CCR per trattare questi incidenti.</t>
+  </si>
+  <si>
+    <t>nm. 59</t>
+  </si>
+  <si>
+    <t>Il trattamento degli incidenti TIC importanti deve essere coordinato e collegato ai processi BCM e DRP.</t>
+  </si>
+  <si>
+    <t>nm. 60</t>
+  </si>
+  <si>
+    <t>Gli incidenti TIC considerati dall’istituto come una perturbazione importante per lo svolgimento dei suoi processi critici e rilevanti ai fini della vigilanza devono essere notificati senza indugio alla FINMA.</t>
+  </si>
+  <si>
+    <t>C. Gestione dei cyber-rischi</t>
+  </si>
+  <si>
+    <t>nm. 61</t>
+  </si>
+  <si>
+    <t>Le aspettative fondamentali poste alla strategia, alla governance e al rafforzamento della consapevolezza in riferimento ai cyber-rischi sono enunciate nei nm. 23–26 e 40.</t>
+  </si>
+  <si>
+    <t>nm. 62</t>
+  </si>
+  <si>
+    <t>L’istituto definisce chiari CCR. Deve coprire almeno gli aspetti seguenti secondo standard e pratiche riconosciuti a livello internazionale e garantire, sviluppare e migliorare conti- nuamente la loro effettiva attuazione mediante procedure, processi e controlli adeguati:</t>
+  </si>
+  <si>
+    <t>nm. 63</t>
+  </si>
+  <si>
+    <t>a. identificazione delle potenziali minacce dovute a cyber-attacchi14 specifiche all’istituto e valutazione delle possibili conseguenze dello sfruttamento delle vulnerabilità relative alle componenti inventariate delle TIC e ai dati elettronici critici (in conformità al nm. 53, 54 e 7);</t>
+  </si>
+  <si>
+    <t>[14] Attacchi alla confidenzialità, all’integrità e alla disponibilità delle TIC, nonché ai dati elettronici critici che si verificano mediante lo sfruttamento delle vulnerabilità o l’elusione delle misure di protezione da parte di aggressori esterni o interni.</t>
+  </si>
+  <si>
+    <t>nm. 64</t>
+  </si>
+  <si>
+    <t>b. protezione delle componenti inventariate delle TIC e dei dati elettronici critici contro i cyber-attacchi mediante l’attuazione di misure di protezione adeguate, in particolare in riferimento alla confidenzialità, all’integrità e alla disponibilità;</t>
+  </si>
+  <si>
+    <t>nm. 65</t>
+  </si>
+  <si>
+    <t>c. individuazione e registrazione tempestive dei cyber-attacchi sulla base di un processo di monitoraggio sistematico e continuo delle componenti inventariate delle TIC e dei dati elettronici critici;</t>
+  </si>
+  <si>
+    <t>nm. 66</t>
+  </si>
+  <si>
+    <t>d. reazione alle vulnerabilità identificate e ai cyber-attacchi mediante lo sviluppo e l’implementazione di processi appropriati, che consentono di adottare tempestivamente misure di attenuazione e di eliminazione; e</t>
+  </si>
+  <si>
+    <t>nm. 67</t>
+  </si>
+  <si>
+    <t>e. garanzia di un rapido ripristino del normale esercizio in seguito a cyber-attacchi con misure appropriate.</t>
+  </si>
+  <si>
+    <t>nm. 68</t>
+  </si>
+  <si>
+    <t>La gestione dei cyber-rischi deve garantire che un cyber-attacco riuscito o parzialmente riuscito sia analizzato in base alla sua rilevanza per le componenti critiche inventariate delle TIC e i dati elettronici critici, nonché i processi critici (incl. i servizi e le funzioni esternalizzati) e che l’obbligo di comunicazione secondo la LFINMA sia rispettato. Dopo una prima valutazione e un’informazione preliminare al servizio competente della FINMA entro 24 ore, la comunicazione deve essere trasmessa entro 72 ore in conformità all’elenco dei requisiti della Piattaforma di rilevamento EHP (campi obbligatori). Una volta che l’istituto ha concluso la trattazione del caso, deve essere presentato al servizio competente della FINMA un rapporto conclusivo sulle cause commisurato al grado di gravità.</t>
+  </si>
+  <si>
+    <t>nm. 69</t>
+  </si>
+  <si>
+    <t>La direzione dispone regolarmente lo svolgimento di analisi di vulnerabilità15 e test di intrusione (penetration test)16, che devono essere eseguiti da personale qualificato con risorse adeguate. In proposito occorre considerare tutte le componenti inventariate delle TIC accessibili tramite internet. Inoltre, devono essere considerate le componenti inventariate delle TIC non accessibili tramite internet, ma necessarie per lo svolgimento di processi critici o contenenti dati elettronici critici.</t>
+  </si>
+  <si>
+    <t>[15] Analisi volta a identificare le vulnerabilità esistenti a livello di software e le falle di sicurezza nell’infrastruttura IT nei confronti di cyber-attacchi.
+[16] Esame mirato e sfruttamento delle vulnerabilità a livello di software e delle falle di sicurezza nelle TIC.</t>
+  </si>
+  <si>
+    <t>nm. 70</t>
+  </si>
+  <si>
+    <t>Sulla base delle minacce potenziali specifiche all’istituto, devono essere svolti cyberesercizi in funzione dei rischi e riferiti allo scenario in questione17. Il risultato degli esercizi deve essere documentato facendone rapporto in forma adeguata.</t>
+  </si>
+  <si>
+    <t>[17] Considerando il nm. 19, questi cyber-esercizi potrebbero includere, per esempio, esercizi di simulazione (table-top exercises), red teaming ecc.</t>
+  </si>
+  <si>
+    <t>D. Gestione dei rischi dei dati critici</t>
+  </si>
+  <si>
+    <t>nm. 71</t>
+  </si>
+  <si>
+    <t>Le aspettative fondamentali poste alla strategia, alla governance e al rafforzamento della consapevolezza in riferimento ai rischi dei dati critici sono enunciate nei nm. 23–26.</t>
+  </si>
+  <si>
+    <t>nm. 72</t>
+  </si>
+  <si>
+    <t>La direzione definisce processi, procedure e controlli adeguati nonché chiari CCR concernenti la gestione dei dati critici individuati dall’istituto. Inoltre, la direzione designa un’unità preposta alla creazione di condizioni quadro che garantiscano la confidenzialità, l’integrità e la disponibilità di dati critici e al controllo del loro rispetto.</t>
+  </si>
+  <si>
+    <t>nm. 73</t>
+  </si>
+  <si>
+    <t>L’istituto individua i suoi dati critici in modo sistematico ed esaustivo, li categorizza in funzione del loro grado di criticità e definisce chiare responsabilità in materia di dati.</t>
+  </si>
+  <si>
+    <t>nm. 74</t>
+  </si>
+  <si>
+    <t>I dati critici definiti dall’istituto sono gestiti lungo il loro intero ciclo di vita.</t>
+  </si>
+  <si>
+    <t>nm. 75</t>
+  </si>
+  <si>
+    <t>Al riguardo, il rispetto della confidenzialità, dell’integrità e della disponibilità nella gestione di dati critici è garantito mediante processi, procedure e controlli adeguati.</t>
+  </si>
+  <si>
+    <t>nm. 76</t>
+  </si>
+  <si>
+    <t>Nell’esercizio e durante lo sviluppo, il cambiamento e la migrazione delle TIC, i dati critici devono essere protetti dall’accesso e dall’utilizzo da parte di soggetti non autorizzati. Questo vale anche per i dati critici in ambienti di test.</t>
+  </si>
+  <si>
+    <t>nm. 77</t>
+  </si>
+  <si>
+    <t>In particolare devono essere protette le componenti delle TIC in cui sono archiviati o trattati dati critici. È necessario regolamentare sistematicamente e monitorare continuamente l’accesso a questi dati.</t>
+  </si>
+  <si>
+    <t>nm. 78</t>
+  </si>
+  <si>
+    <t>L’accesso ai dati critici e alle funzioni legate al trattamento di questi dati è limitato alle persone che necessitano dei dati per svolgere i propri compiti18. Al riguardo l’istituto deve disporre di un sistema di autorizzazione. L’accesso a tale sistema di autorizzazione deve essere protetto in modo particolare e verificato regolarmente. Le autorizzazioni contenute nel sistema devono essere verificate regolarmente.</t>
+  </si>
+  <si>
+    <t>[18] P. es. principio del need-to-know e del privilegio minimo (least privilege).</t>
+  </si>
+  <si>
+    <t>nm. 79</t>
+  </si>
+  <si>
+    <t>Se i dati critici sono archiviati al di fuori della Svizzera19 o sono accessibili dall’estero, è necessario limitare adeguatamente i rischi superiori che ne derivano e monitorarli mediante misure adeguate, nonché proteggere i dati in modo particolare.</t>
+  </si>
+  <si>
+    <t>[19] P. es. mediante soluzioni di cloud o di hosting.</t>
+  </si>
+  <si>
+    <t>nm. 80</t>
+  </si>
+  <si>
+    <t>Occorre scegliere accuratamente le persone interne e quelle esterne che possono accedere ai dati critici o modificarli. Tali persone devono essere sorvegliate mediante misure appropriate20 e formate regolarmente sulla gestione di questi dati. Alle persone che beneficiano di maggiori privilegi21 si applicano requisiti di sicurezza più rigorosi. Inoltre, deve essere tenuto un elenco di tutte le persone che beneficiano di maggiori privilegi e aggiornato continuamente.</t>
+  </si>
+  <si>
+    <t>[20] P. es. valutazione di file log, principio del doppio controllo ecc.
+[21] P. es. persone con diritti di amministratore, utenti con accesso funzionale a una grossa quantità di dati critici ecc.</t>
+  </si>
+  <si>
+    <t>nm. 81</t>
+  </si>
+  <si>
+    <t>Gli incidenti che compromettono in misura significativa la confidenzialità, l’integrità o la disponibilità di dati critici devono essere notificati senza indugio alla FINMA.</t>
+  </si>
+  <si>
+    <t>nm. 82</t>
+  </si>
+  <si>
+    <t>Nella scelta dei fornitori di servizi che trattano dati critici22 o possono consultarli deve essere attribuita una notevole importanza alla verifica della diligenza (due diligence). Occorre definire criteri chiari per valutare il modo in cui i fornitori di servizi gestiscono dati critici ed esaminarlo prima di firmare i contratti. I fornitori di servizi devono essere sottoposti a un monitoraggio e a un controllo periodici nell’ambito del sistema di controllo interno dell’istituto.</t>
+  </si>
+  <si>
+    <t>[22] Trattamento: qualunque modo di gestire dati critici, a prescindere dai mezzi e dalle procedure impiegati, in particolare l’acquisizione, il salvataggio, la custodia, l’utilizzo, la modifica, la divulgazione, l’archiviazione, la cancellazione o l’eliminazione dei dati.</t>
+  </si>
+  <si>
+    <t>nm. 83</t>
+  </si>
+  <si>
+    <t>Le aspettative fondamentali poste alla strategia, alla governance e al rafforzamento della consapevolezza in riferimento ai rischi che derivano dalla configurazione e dall’implementazione del BCM sono enunciate nei nm. 23–26.</t>
+  </si>
+  <si>
+    <t>nm. 84</t>
+  </si>
+  <si>
+    <t>Ogni divisione operativa e organizzativa rilevante deve individuare i suoi processi critici e le risorse necessarie23 nell’ambito della business impact analysis (BIA).</t>
+  </si>
+  <si>
+    <t>[23] Personale, infrastrutture (p. es. immobili, infrastruttura dei posti di lavoro), informazioni, sistemi IT o infrastruttura IT (compresi i sistemi di comunicazione), dipendenze da altri settori dell’istituto e da terzi, p. es. erogatori di servizi e fornitori esterni (outsourcing), banche centrali o stanze di compensazione.</t>
+  </si>
+  <si>
+    <t>nm. 85</t>
+  </si>
+  <si>
+    <t>Per i processi critici, l’istituto definisce il RTO e il RPO secondo il nm. 10, coordinandoli con i necessari fornitori di servizi24. La loro osservanza è disciplinata mediante service level agreement o contratti, oppure è garantita mediante procedure, processi e controlli appropriati.</t>
+  </si>
+  <si>
+    <t>[24] P. es. con la sezione IT, altre divisioni dell’istituto o esterni.</t>
+  </si>
+  <si>
+    <t>nm. 86</t>
+  </si>
+  <si>
+    <t>L’istituto definisce almeno un BCP secondo il nm. 11, che descrive anche gli eventi che comportano l’attivazione del piano e i processi decisionali e tiene conto della perdita di risorse secondo il nm. 84. I rischi residui accettati sono documentati in maniera adeguata.</t>
+  </si>
+  <si>
+    <t>nm. 87</t>
+  </si>
+  <si>
+    <t>La BIA e il BCP sono allestiti e documentati in modo sistematico secondo una direttiva applicabile a tutto l’istituto. Devono essere verificati e aggiornati ogni anno e ad hoc in caso di cambiamenti sostanziali nell’attività (riorganizzazioni, creazione di un nuovo campo di attività ecc.).</t>
+  </si>
+  <si>
+    <t>nm. 88</t>
+  </si>
+  <si>
+    <t>L’istituto definisce almeno un DRP come parte integrante del BCP. Se vengono esternalizzati processi critici o singole parti di essi, il DRP tiene conto delle dipendenze interne e delle disposizioni contrattuali nonché di soluzioni alternative. Il DRP è verificato e aggiornato ad hoc in caso di cambiamenti sostanziali, ma almeno una volta all’anno.</t>
+  </si>
+  <si>
+    <t>nm. 89</t>
+  </si>
+  <si>
+    <t>Nelle situazioni di crisi, uno stato maggiore di crisi è incaricato di gestire la crisi fino al ripristino della situazione conforme. Gli eventi che scatenano una crisi e i CCR dello stato maggiore di crisi devono essere previamente regolamentati e l’organizzazione di crisi deve essere incentrata sull’attività commerciale e la struttura geografica dell’istituto. Nelle situazioni di crisi deve essere garantita la reperibilità dei responsabili.</t>
+  </si>
+  <si>
+    <t>nm. 90</t>
+  </si>
+  <si>
+    <t>L’istituto definisce una strategia di comunicazione interna ed esterna nelle situazioni di crisi.</t>
+  </si>
+  <si>
+    <t>nm. 91</t>
+  </si>
+  <si>
+    <t>L’attuazione del BCP e del DRP e la funzionalità dell’organizzazione di crisi sono regolarmente valutate. A tal fine l’istituto appronta una pianificazione sistematica dei test che garantisce la copertura regolare. È possibile scegliere diverse modalità di test con gradi di intensità e di efficacia variabile, per esempio gli esercizi table-top.</t>
+  </si>
+  <si>
+    <t>nm. 92</t>
+  </si>
+  <si>
+    <t>Le principali misure in conformità al BCP e al DRP e l’organizzazione di crisi sono testate almeno una volta all’anno.</t>
+  </si>
+  <si>
+    <t>nm. 93</t>
+  </si>
+  <si>
+    <t>I principali stakeholder, compresi quelli che svolgono funzioni specialistiche e IT, partecipano ai test per acquisire dimestichezza con i processi di ripristino.</t>
+  </si>
+  <si>
+    <t>nm. 94</t>
+  </si>
+  <si>
+    <t>I test comprendono scenari di diversa gravità, ma plausibili e considerano le dipendenze ai fini del ripristino, comprese quelle nei confronti di terzi interni o esterni.</t>
+  </si>
+  <si>
+    <t>nm. 95</t>
+  </si>
+  <si>
+    <t>Resoconti periodici all’organo preposto all’alta direzione e alla direzione informano in merito alle attività di test e di verifica condotte e ai relativi risultati. Presentano chiaramente le priorità adottate (p. es. gerarchia delle priorità dei processi critici necessari per l’esecuzione delle funzioni critiche secondo il nm. 14) e le lacune individuate nella copertura di altri processi critici.</t>
+  </si>
+  <si>
+    <t>nm. 96</t>
+  </si>
+  <si>
+    <t>I collaboratori e i membri dell’organizzazione di crisi sono adeguatamente preparati riguardo ai loro CCR riconducibili alle diverse attività di BCM sia al momento dell’entrata in servizio sia nel corso delle formazioni periodiche.</t>
+  </si>
+  <si>
+    <t>F. Gestione dei rischi afferenti alle prestazioni di servizio transfrontaliere</t>
+  </si>
+  <si>
+    <t>nm. 97</t>
+  </si>
+  <si>
+    <t>Se gli istituti o le società del gruppo forniscono servizi o distribuiscono prodotti finanziari oltrefrontiera, anche i rischi risultanti dall’applicazione delle normative estere (diritto fiscale, penale, in materia di riciclaggio di denaro ecc.) devono essere adeguatamente rilevati, limitati e controllati.</t>
+  </si>
+  <si>
+    <t>nm. 98</t>
+  </si>
+  <si>
+    <t>Gli istituti sottopongono le loro prestazioni di servizio transfrontaliere e la distribuzione transfrontaliera di prodotti finanziari a un’analisi approfondita delle condizioni quadro giuridiche e dei rischi correlati. Sulla base di questa analisi, gli istituti adottano le necessarie misure strategiche e organizzative volte a eliminare e minimizzare i rischi e le adeguano continuamente all’evolversi della situazione. In particolare dispongono delle necessarie competenze specialistiche specifiche ai vari Paesi, definiscono specifici modelli di servizi per i Paesi in cui li erogano, formano i collaboratori e garantiscono l’osservanza delle prescrizioni mediante misure organizzative, direttive, modelli retributivi e sanzionatori.</t>
+  </si>
+  <si>
+    <t>nm. 99</t>
+  </si>
+  <si>
+    <t>È necessario considerare anche i rischi generati da gestori patrimoniali indipendenti, intermediari e altri fornitori di servizi. I partner devono essere scelti e formati con l’opportuna accuratezza.</t>
+  </si>
+  <si>
+    <t>nm. 100</t>
+  </si>
+  <si>
+    <t>Questo principio si applica pure alle situazioni in cui una filiale, una succursale o un’entità simile con sede all’estero di un istituto finanziario svizzero fornisce servizi transfrontalieri ai clienti.</t>
+  </si>
+  <si>
+    <t>V. Garanzia della resilienza operativa</t>
+  </si>
+  <si>
+    <t>nm. 101</t>
+  </si>
+  <si>
+    <t>L’istituto identifica le sue funzioni critiche e i rispettivi limiti di tolleranza alle interruzioni, che sono approvati dall’organo preposto all’alta direzione. Inoltre, l’organo preposto all’alta direzione approva e sorveglia regolarmente la procedura volta a garantire la resilienza operativa.</t>
+  </si>
+  <si>
+    <t>nm. 102</t>
+  </si>
+  <si>
+    <t>L’istituto adotta misure per garantire la resilienza operativa considerando scenari gravi, ma plausibili25.</t>
+  </si>
+  <si>
+    <t>[25] Non si può escludere che alcuni scenari non possano essere fronteggiati senza il coinvolgimento dello Stato (p. es. pandemie, guerre, persistente penuria di energia). In tali casi l’istituto deve svolgere lavori preliminari volti a raffor- zare la sua resilienza operativa nei confronti di questi scenari nell’ambito delle sue possibilità.</t>
+  </si>
+  <si>
+    <t>nm. 103</t>
+  </si>
+  <si>
+    <t>Le funzioni critiche e i correlati limiti di tolleranza alle interruzioni secondo il nm. 14 devono essere approvati dall’organo preposto all’alta direzione almeno una volta all’anno.</t>
+  </si>
+  <si>
+    <t>nm. 104</t>
+  </si>
+  <si>
+    <t>L’istituto coordina le principali componenti di una gestione completa del rischio, per esempio la gestione dei rischi operativi, inclusa la gestione del rischi TIC e dei cyber-rischi, il business continuity management, la gestione delle esternalizzazioni (outsourcing; cfr. Circ. FINMA 18/3 «Outsourcing») e la pianificazione d’emergenza (capitolo VI), affinché contribuiscano a rafforzare la resilienza operativa dell’istituto. Ciò include uno scambio adeguato delle informazioni rilevanti tra i diversi ambiti.</t>
+  </si>
+  <si>
+    <t>nm. 105</t>
+  </si>
+  <si>
+    <t>L’organo preposto all’alta direzione e la direzione devono ricevere almeno una volta all’anno un resoconto sulla resilienza operativa, nonché in caso di lacune sostanziali nei controlli o di incidenti che compromettono la resilienza operativa.</t>
+  </si>
+  <si>
+    <t>nm. 106</t>
+  </si>
+  <si>
+    <t>Per le funzioni critiche si procede a identificare e valutare le minacce interne ed esterne come pure lo sfruttamento delle vulnerabilità. I risultanti rischi operativi sono identificati, valutati, limitati e monitorati nell’ambito della loro gestione.</t>
+  </si>
+  <si>
+    <t>nm. 107</t>
+  </si>
+  <si>
+    <t>L’istituto tiene un inventario delle sue funzioni critiche da verificare e aggiornare almeno una volta all’anno. Tale inventario contiene le tolleranze alle interruzioni delle funzioni critiche, nonché i collegamenti e le dipendenze tra i processi critici necessari e le relative risorse26 per svolgere le funzioni critiche.</t>
+  </si>
+  <si>
+    <t>[26] Incluse le componenti dell’inventario rilevanti per le funzioni critiche secondo il nm. 53.</t>
+  </si>
+  <si>
+    <t>nm. 108</t>
+  </si>
+  <si>
+    <t>Per le funzioni critiche sono documentati almeno i rischi operativi essenziali e i controlli chiave.</t>
+  </si>
+  <si>
+    <t>nm. 109</t>
+  </si>
+  <si>
+    <t>Le funzioni critiche nonché le risorse e i processi critici necessari alla loro esecuzione sono coperti dai BCP secondo il capitolo IV. lettera e.</t>
+  </si>
+  <si>
+    <t>nm. 110</t>
+  </si>
+  <si>
+    <t>La capacità di eseguire funzioni critiche entro i loro limiti di tolleranza alle interruzioni in scenari gravi, ma plausibili è regolarmente testata o esercitata. Ciò comprende anche gli scenari che si differenziano dalle interruzioni brevi e con un effetto piuttosto limitato e sono caratterizzati da una durata prolungata (p. es. diversi mesi) e dall’insufficienza delle risorse fondamentali27. I test e gli esercizi sono configurati in modo tale da non costituire una minaccia sostanziale per l’istituto.</t>
+  </si>
+  <si>
+    <t>[27] Tra gli altri, una pandemia, una penuria di energia, un’insufficienza prolungata ascrivibile all’insolvenza di un impor- tante fornitore di servizi (p. es. con conseguente ritiro da un accordo di outsourcing) o un divieto prolungato da parte di governi stranieri, in base al quale i fornitori di servizi cloud o altri fornitori di servizi con sede all’estero non sono più autorizzati a erogare servizi alle società svizzere.</t>
+  </si>
+  <si>
+    <t>nm. 111</t>
+  </si>
+  <si>
+    <t>Per le banche di rilevanza sistemica, il BCP, il DRP e l’organizzazione di crisi in conformità al capitolo IV. lett. E., rilevanti per il mantenimento delle funzioni critiche secondo il nm. 14, devono essere coordinati con la pianificazione d’emergenza in conformità al capitolo VI.</t>
+  </si>
+  <si>
+    <t>VI. Mantenimento dei servizi critici in caso di liquidazione o risanamento delle banche di rilevanza sistemica</t>
+  </si>
+  <si>
+    <t>nm. 112</t>
+  </si>
+  <si>
+    <t>Nel quadro della loro pianificazione d’emergenza, le banche di rilevanza sistemica adottano le misure necessarie per garantire il mantenimento senza interruzioni delle funzioni di rilevanza sistemica (art. 9 cpv. 2 lett. d LBCR in combinato disposto con l’art. 60 segg. OBCR). Identificano i servizi essenziali per il mantenimento delle funzioni di rilevanza sistemica in caso di liquidazione, risanamento o ristrutturazione («servizi critici») e adottano le misure necessarie a tale scopo. Al riguardo tengono conto delle disposizioni emanate in materia dagli organismi internazionali di standardizzazione.</t>
+  </si>
+  <si>
+    <t>VII. Disposizioni transitorie</t>
+  </si>
+  <si>
+    <t>A. Concernenti la garanzia della resilienza operativa</t>
+  </si>
+  <si>
+    <t>nm. 113</t>
+  </si>
+  <si>
+    <t>L’identificazione delle funzioni critiche, la definizione della tolleranza alle interruzioni e le prime approvazioni in conformità ai nm. 101 e 103, nonché un primo resoconto secondo il nm. 105 sono attesi a partire dall’entrata in vigore della presente circolare. Per l’adempimento dei requisiti di cui ai nm. 106–109 e i primi test secondo il nm. 110 è accordato un termine transitorio di un anno dall’entrata in vigore. La garanzia della resilienza operativa in conformità al nm. 102 e l’adempimento dei requisiti di cui ai nm. 104 e 111 sono attesi entro un termine transitorio di due anni.</t>
+  </si>
+  <si>
+    <t>B. Concernenti le esigenze in materia di fondi propri per la copertura dei rischi operativi</t>
+  </si>
+  <si>
+    <t>nm. 114</t>
+  </si>
+  <si>
+    <t>Le esigenze in materia di fondi propri per i rischi operativi ai sensi degli artt. 89 segg. OFoP sono rette dai nm. 3–116 della Circolare FINMA 08/21 «Rischi operativi – banche» sino all’entrata in vigore dell’OFoP riveduta nel quadro del pacchetto di revisioni «Basilea III finale» e della relativa ordinanza esecutiva della FINMA.</t>
+  </si>
+  <si>
+    <t>FINMA - Circolare 2023/01 - Rischi operativi e resilienza - Banche</t>
+  </si>
+  <si>
+    <t>Gestione dei rischi operativi e garanzia della resilienza ope- rativa
+Riferimento: Circ. FINMA 23/1 «Rischi operativi e resilienza – banche»
+Data: 7 dicembre 2022
+Entrata in vigore: 1° gennaio 2024
+Concordanza: sostituisce la Circ. FINMA 08/21 «Rischi operativi – banche» del 20 novembre 2008
+Basi legali: LFINMA art. 7 cpv. 1 lett. b e art. 29 cpv. 1
+                     LBCR art. 1b cpv. 3 lett. b, art. 3 cpv. 2 lett. a e art. 3f
+                     OBCR artt. 12 e 14e
+                     LIsFi artt. 9 e 49
+                     OIsFi artt. 12 e 68</t>
   </si>
 </sst>
 </file>
@@ -1813,14 +2648,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2123,10 +2956,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD9"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2208,35 +3041,51 @@
       </c>
       <c r="C9" s="1"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>574</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>575</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>847</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B15" s="2" t="s">
         <v>457</v>
       </c>
     </row>
@@ -2247,15 +3096,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD8"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="95.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -2314,7 +3164,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>300</v>
       </c>
@@ -2322,6 +3172,22 @@
         <v>459</v>
       </c>
       <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>574</v>
+      </c>
+      <c r="B9" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>575</v>
+      </c>
+      <c r="B10" t="s">
+        <v>847</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2330,23 +3196,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:I134"/>
+  <dimension ref="A1:L134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H134" sqref="H134"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="5" max="5" width="114.88671875" customWidth="1"/>
     <col min="6" max="6" width="75.33203125" customWidth="1"/>
-    <col min="7" max="7" width="20.109375" customWidth="1"/>
+    <col min="7" max="7" width="15" customWidth="1"/>
     <col min="8" max="8" width="142" style="1" customWidth="1"/>
     <col min="9" max="9" width="78.21875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="8.33203125" customWidth="1"/>
+    <col min="11" max="11" width="157.44140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="67.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>24</v>
       </c>
@@ -2374,8 +3243,17 @@
       <c r="I1" s="1" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J1" t="s">
+        <v>574</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B2">
         <v>1</v>
       </c>
@@ -2387,8 +3265,11 @@
       <c r="G2" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J2" t="s">
+        <v>577</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B3">
         <v>2</v>
       </c>
@@ -2410,8 +3291,17 @@
       <c r="I3" s="1" t="s">
         <v>304</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J3" t="s">
+        <v>578</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>579</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>2</v>
       </c>
@@ -2428,8 +3318,14 @@
       <c r="H4" s="1" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J4" t="s">
+        <v>581</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>1</v>
       </c>
@@ -2441,8 +3337,11 @@
       <c r="G5" t="s">
         <v>306</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="J5" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>2</v>
       </c>
@@ -2464,8 +3363,17 @@
       <c r="I6" s="1" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J6" t="s">
+        <v>584</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B7">
         <v>2</v>
       </c>
@@ -2482,8 +3390,14 @@
       <c r="H7" s="1" t="s">
         <v>309</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J7" t="s">
+        <v>587</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>2</v>
       </c>
@@ -2500,8 +3414,14 @@
       <c r="H8" s="1" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J8" t="s">
+        <v>589</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>2</v>
       </c>
@@ -2518,8 +3438,14 @@
       <c r="H9" s="1" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="J9" t="s">
+        <v>591</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>2</v>
       </c>
@@ -2536,8 +3462,14 @@
       <c r="H10" s="1" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J10" t="s">
+        <v>593</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>2</v>
       </c>
@@ -2554,8 +3486,14 @@
       <c r="H11" s="1" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J11" t="s">
+        <v>595</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>2</v>
       </c>
@@ -2572,8 +3510,14 @@
       <c r="H12" s="1" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J12" t="s">
+        <v>597</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>2</v>
       </c>
@@ -2590,8 +3534,14 @@
       <c r="H13" s="1" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J13" t="s">
+        <v>599</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B14">
         <v>2</v>
       </c>
@@ -2608,8 +3558,14 @@
       <c r="H14" s="1" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J14" t="s">
+        <v>601</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>2</v>
       </c>
@@ -2626,8 +3582,14 @@
       <c r="H15" s="1" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J15" t="s">
+        <v>603</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>2</v>
       </c>
@@ -2644,8 +3606,14 @@
       <c r="H16" s="1" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J16" t="s">
+        <v>605</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>2</v>
       </c>
@@ -2662,8 +3630,14 @@
       <c r="H17" s="1" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J17" t="s">
+        <v>607</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>2</v>
       </c>
@@ -2680,8 +3654,14 @@
       <c r="H18" s="1" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J18" t="s">
+        <v>609</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>2</v>
       </c>
@@ -2698,8 +3678,14 @@
       <c r="H19" s="1" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J19" t="s">
+        <v>611</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B20">
         <v>2</v>
       </c>
@@ -2716,8 +3702,14 @@
       <c r="H20" s="1" t="s">
         <v>322</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="J20" t="s">
+        <v>613</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="B21">
         <v>2</v>
       </c>
@@ -2739,8 +3731,17 @@
       <c r="I21" s="1" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J21" t="s">
+        <v>615</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>616</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B22">
         <v>1</v>
       </c>
@@ -2752,8 +3753,11 @@
       <c r="G22" t="s">
         <v>325</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J22" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B23">
         <v>2</v>
       </c>
@@ -2770,8 +3774,14 @@
       <c r="H23" s="1" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J23" t="s">
+        <v>619</v>
+      </c>
+      <c r="K23" s="1" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B24">
         <v>2</v>
       </c>
@@ -2788,8 +3798,14 @@
       <c r="H24" s="1" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J24" t="s">
+        <v>621</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B25">
         <v>2</v>
       </c>
@@ -2806,8 +3822,14 @@
       <c r="H25" s="1" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J25" t="s">
+        <v>623</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B26">
         <v>1</v>
       </c>
@@ -2819,8 +3841,11 @@
       <c r="G26" t="s">
         <v>329</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J26" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B27">
         <v>2</v>
       </c>
@@ -2832,8 +3857,11 @@
       <c r="G27" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J27" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B28">
         <v>3</v>
       </c>
@@ -2850,8 +3878,14 @@
       <c r="H28" s="1" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="J28" t="s">
+        <v>627</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>79</v>
       </c>
@@ -2876,8 +3910,17 @@
       <c r="I29" s="1" t="s">
         <v>333</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J29" t="s">
+        <v>629</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>79</v>
       </c>
@@ -2897,8 +3940,14 @@
       <c r="H30" s="1" t="s">
         <v>334</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J30" t="s">
+        <v>632</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>79</v>
       </c>
@@ -2923,8 +3972,17 @@
       <c r="I31" s="1" t="s">
         <v>336</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J31" t="s">
+        <v>634</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="L31" s="1" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>79</v>
       </c>
@@ -2949,8 +4007,17 @@
       <c r="I32" s="1" t="s">
         <v>338</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J32" t="s">
+        <v>637</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>638</v>
+      </c>
+      <c r="L32" s="1" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>79</v>
       </c>
@@ -2970,8 +4037,14 @@
       <c r="H33" s="1" t="s">
         <v>339</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J33" t="s">
+        <v>640</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>79</v>
       </c>
@@ -2991,8 +4064,14 @@
       <c r="H34" s="1" t="s">
         <v>340</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="J34" t="s">
+        <v>642</v>
+      </c>
+      <c r="K34" s="1" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>79</v>
       </c>
@@ -3017,8 +4096,17 @@
       <c r="I35" s="1" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J35" t="s">
+        <v>644</v>
+      </c>
+      <c r="K35" s="1" t="s">
+        <v>645</v>
+      </c>
+      <c r="L35" s="1" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>79</v>
       </c>
@@ -3043,8 +4131,17 @@
       <c r="I36" s="1" t="s">
         <v>344</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J36" t="s">
+        <v>647</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="L36" s="1" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>79</v>
       </c>
@@ -3064,8 +4161,14 @@
       <c r="H37" s="1" t="s">
         <v>345</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J37" t="s">
+        <v>650</v>
+      </c>
+      <c r="K37" s="1" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>79</v>
       </c>
@@ -3085,8 +4188,14 @@
       <c r="H38" s="1" t="s">
         <v>346</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J38" t="s">
+        <v>652</v>
+      </c>
+      <c r="K38" s="1" t="s">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>79</v>
       </c>
@@ -3106,8 +4215,14 @@
       <c r="H39" s="1" t="s">
         <v>347</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J39" t="s">
+        <v>654</v>
+      </c>
+      <c r="K39" s="1" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>79</v>
       </c>
@@ -3127,8 +4242,14 @@
       <c r="H40" s="1" t="s">
         <v>348</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J40" t="s">
+        <v>656</v>
+      </c>
+      <c r="K40" s="1" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>79</v>
       </c>
@@ -3148,8 +4269,14 @@
       <c r="H41" s="1" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J41" t="s">
+        <v>658</v>
+      </c>
+      <c r="K41" s="1" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>79</v>
       </c>
@@ -3169,8 +4296,14 @@
       <c r="H42" s="1" t="s">
         <v>350</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J42" t="s">
+        <v>660</v>
+      </c>
+      <c r="K42" s="1" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>79</v>
       </c>
@@ -3190,8 +4323,14 @@
       <c r="H43" s="1" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="J43" t="s">
+        <v>662</v>
+      </c>
+      <c r="K43" s="1" t="s">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>79</v>
       </c>
@@ -3216,8 +4355,17 @@
       <c r="I44" s="1" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J44" t="s">
+        <v>664</v>
+      </c>
+      <c r="K44" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="L44" s="1" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>79</v>
       </c>
@@ -3242,8 +4390,17 @@
       <c r="I45" s="1" t="s">
         <v>355</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J45" t="s">
+        <v>667</v>
+      </c>
+      <c r="K45" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="L45" s="1" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>79</v>
       </c>
@@ -3263,8 +4420,14 @@
       <c r="H46" s="1" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J46" t="s">
+        <v>670</v>
+      </c>
+      <c r="K46" s="1" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>79</v>
       </c>
@@ -3284,8 +4447,14 @@
       <c r="H47" s="1" t="s">
         <v>357</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J47" t="s">
+        <v>672</v>
+      </c>
+      <c r="K47" s="1" t="s">
+        <v>673</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>79</v>
       </c>
@@ -3305,8 +4474,14 @@
       <c r="H48" s="1" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J48" t="s">
+        <v>674</v>
+      </c>
+      <c r="K48" s="1" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>79</v>
       </c>
@@ -3326,8 +4501,14 @@
       <c r="H49" s="1" t="s">
         <v>359</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J49" t="s">
+        <v>676</v>
+      </c>
+      <c r="K49" s="1" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>79</v>
       </c>
@@ -3347,8 +4528,14 @@
       <c r="H50" s="1" t="s">
         <v>360</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J50" t="s">
+        <v>678</v>
+      </c>
+      <c r="K50" s="1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>79</v>
       </c>
@@ -3368,8 +4555,14 @@
       <c r="H51" s="1" t="s">
         <v>361</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J51" t="s">
+        <v>680</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>79</v>
       </c>
@@ -3389,8 +4582,14 @@
       <c r="H52" s="1" t="s">
         <v>362</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J52" t="s">
+        <v>682</v>
+      </c>
+      <c r="K52" s="1" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B53">
         <v>2</v>
       </c>
@@ -3402,11 +4601,11 @@
       <c r="G53" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A54" t="s">
-        <v>79</v>
-      </c>
+      <c r="J53" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B54">
         <v>3</v>
       </c>
@@ -3418,8 +4617,11 @@
       <c r="G54" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J54" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>79</v>
       </c>
@@ -3439,8 +4641,14 @@
       <c r="H55" s="1" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J55" t="s">
+        <v>686</v>
+      </c>
+      <c r="K55" s="1" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="56" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>79</v>
       </c>
@@ -3460,8 +4668,14 @@
       <c r="H56" s="1" t="s">
         <v>366</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J56" t="s">
+        <v>688</v>
+      </c>
+      <c r="K56" s="1" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>79</v>
       </c>
@@ -3481,11 +4695,14 @@
       <c r="H57" s="1" t="s">
         <v>367</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A58" t="s">
-        <v>79</v>
-      </c>
+      <c r="J57" t="s">
+        <v>690</v>
+      </c>
+      <c r="K57" s="1" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B58">
         <v>3</v>
       </c>
@@ -3497,8 +4714,11 @@
       <c r="G58" t="s">
         <v>368</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J58" t="s">
+        <v>692</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>79</v>
       </c>
@@ -3518,8 +4738,14 @@
       <c r="H59" s="1" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J59" t="s">
+        <v>693</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>79</v>
       </c>
@@ -3539,8 +4765,14 @@
       <c r="H60" s="1" t="s">
         <v>370</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J60" t="s">
+        <v>695</v>
+      </c>
+      <c r="K60" s="1" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>79</v>
       </c>
@@ -3565,8 +4797,17 @@
       <c r="I61" s="1" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J61" t="s">
+        <v>697</v>
+      </c>
+      <c r="K61" s="1" t="s">
+        <v>698</v>
+      </c>
+      <c r="L61" s="1" t="s">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B62">
         <v>3</v>
       </c>
@@ -3578,8 +4819,11 @@
       <c r="G62" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="63" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J62" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>79</v>
       </c>
@@ -3599,8 +4843,14 @@
       <c r="H63" s="1" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J63" t="s">
+        <v>701</v>
+      </c>
+      <c r="K63" s="1" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>79</v>
       </c>
@@ -3620,8 +4870,14 @@
       <c r="H64" s="1" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="65" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J64" t="s">
+        <v>703</v>
+      </c>
+      <c r="K64" s="1" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>79</v>
       </c>
@@ -3641,8 +4897,14 @@
       <c r="H65" s="1" t="s">
         <v>376</v>
       </c>
-    </row>
-    <row r="66" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J65" t="s">
+        <v>705</v>
+      </c>
+      <c r="K65" s="1" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>79</v>
       </c>
@@ -3662,8 +4924,14 @@
       <c r="H66" s="1" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J66" t="s">
+        <v>707</v>
+      </c>
+      <c r="K66" s="1" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>79</v>
       </c>
@@ -3683,8 +4951,14 @@
       <c r="H67" s="1" t="s">
         <v>378</v>
       </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J67" t="s">
+        <v>709</v>
+      </c>
+      <c r="K67" s="1" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B68">
         <v>3</v>
       </c>
@@ -3696,8 +4970,11 @@
       <c r="G68" t="s">
         <v>379</v>
       </c>
-    </row>
-    <row r="69" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J68" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>79</v>
       </c>
@@ -3717,8 +4994,14 @@
       <c r="H69" s="1" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J69" t="s">
+        <v>712</v>
+      </c>
+      <c r="K69" s="1" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>79</v>
       </c>
@@ -3738,8 +5021,14 @@
       <c r="H70" s="1" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J70" t="s">
+        <v>714</v>
+      </c>
+      <c r="K70" s="1" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>79</v>
       </c>
@@ -3759,8 +5048,14 @@
       <c r="H71" s="1" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J71" t="s">
+        <v>716</v>
+      </c>
+      <c r="K71" s="1" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B72">
         <v>2</v>
       </c>
@@ -3772,8 +5067,11 @@
       <c r="G72" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="73" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J72" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>79</v>
       </c>
@@ -3793,8 +5091,14 @@
       <c r="H73" s="1" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="74" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J73" t="s">
+        <v>719</v>
+      </c>
+      <c r="K73" s="1" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>79</v>
       </c>
@@ -3814,8 +5118,14 @@
       <c r="H74" s="1" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="75" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J74" t="s">
+        <v>721</v>
+      </c>
+      <c r="K74" s="1" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>79</v>
       </c>
@@ -3840,8 +5150,17 @@
       <c r="I75" s="1" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="76" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J75" t="s">
+        <v>723</v>
+      </c>
+      <c r="K75" s="1" t="s">
+        <v>724</v>
+      </c>
+      <c r="L75" s="1" t="s">
+        <v>725</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>79</v>
       </c>
@@ -3861,8 +5180,14 @@
       <c r="H76" s="1" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="77" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J76" t="s">
+        <v>726</v>
+      </c>
+      <c r="K76" s="1" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>79</v>
       </c>
@@ -3882,8 +5207,14 @@
       <c r="H77" s="1" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J77" t="s">
+        <v>728</v>
+      </c>
+      <c r="K77" s="1" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>79</v>
       </c>
@@ -3903,8 +5234,14 @@
       <c r="H78" s="1" t="s">
         <v>390</v>
       </c>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J78" t="s">
+        <v>730</v>
+      </c>
+      <c r="K78" s="1" t="s">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -3924,8 +5261,14 @@
       <c r="H79" s="1" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="80" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="J79" t="s">
+        <v>732</v>
+      </c>
+      <c r="K79" s="1" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="80" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -3947,8 +5290,14 @@
       <c r="H80" s="1" t="s">
         <v>392</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="J80" t="s">
+        <v>734</v>
+      </c>
+      <c r="K80" s="1" t="s">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>79</v>
       </c>
@@ -3973,8 +5322,17 @@
       <c r="I81" s="1" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J81" t="s">
+        <v>736</v>
+      </c>
+      <c r="K81" s="1" t="s">
+        <v>737</v>
+      </c>
+      <c r="L81" s="1" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -3999,8 +5357,17 @@
       <c r="I82" s="1" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J82" t="s">
+        <v>739</v>
+      </c>
+      <c r="K82" s="1" t="s">
+        <v>740</v>
+      </c>
+      <c r="L82" s="1" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B83">
         <v>2</v>
       </c>
@@ -4012,8 +5379,11 @@
       <c r="G83" t="s">
         <v>397</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J83" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="84" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>79</v>
       </c>
@@ -4033,8 +5403,14 @@
       <c r="H84" s="1" t="s">
         <v>398</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J84" t="s">
+        <v>743</v>
+      </c>
+      <c r="K84" s="1" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>79</v>
       </c>
@@ -4054,8 +5430,14 @@
       <c r="H85" s="1" t="s">
         <v>399</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J85" t="s">
+        <v>745</v>
+      </c>
+      <c r="K85" s="1" t="s">
+        <v>746</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>79</v>
       </c>
@@ -4075,8 +5457,14 @@
       <c r="H86" s="1" t="s">
         <v>400</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J86" t="s">
+        <v>747</v>
+      </c>
+      <c r="K86" s="1" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>79</v>
       </c>
@@ -4096,8 +5484,14 @@
       <c r="H87" s="1" t="s">
         <v>401</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J87" t="s">
+        <v>749</v>
+      </c>
+      <c r="K87" s="1" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>79</v>
       </c>
@@ -4117,8 +5511,14 @@
       <c r="H88" s="1" t="s">
         <v>402</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J88" t="s">
+        <v>751</v>
+      </c>
+      <c r="K88" s="1" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>79</v>
       </c>
@@ -4138,8 +5538,14 @@
       <c r="H89" s="1" t="s">
         <v>403</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J89" t="s">
+        <v>753</v>
+      </c>
+      <c r="K89" s="1" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>79</v>
       </c>
@@ -4159,8 +5565,14 @@
       <c r="H90" s="1" t="s">
         <v>404</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J90" t="s">
+        <v>755</v>
+      </c>
+      <c r="K90" s="1" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>79</v>
       </c>
@@ -4185,8 +5597,17 @@
       <c r="I91" s="1" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J91" t="s">
+        <v>757</v>
+      </c>
+      <c r="K91" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="L91" s="1" t="s">
+        <v>759</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>79</v>
       </c>
@@ -4211,8 +5632,17 @@
       <c r="I92" s="1" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J92" t="s">
+        <v>760</v>
+      </c>
+      <c r="K92" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="L92" s="1" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>79</v>
       </c>
@@ -4237,8 +5667,17 @@
       <c r="I93" s="1" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J93" t="s">
+        <v>763</v>
+      </c>
+      <c r="K93" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="L93" s="1" t="s">
+        <v>765</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>79</v>
       </c>
@@ -4258,8 +5697,14 @@
       <c r="H94" s="1" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J94" t="s">
+        <v>766</v>
+      </c>
+      <c r="K94" s="1" t="s">
+        <v>767</v>
+      </c>
+    </row>
+    <row r="95" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>79</v>
       </c>
@@ -4284,8 +5729,17 @@
       <c r="I95" s="1" t="s">
         <v>413</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J95" t="s">
+        <v>768</v>
+      </c>
+      <c r="K95" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="L95" s="1" t="s">
+        <v>770</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B96">
         <v>2</v>
       </c>
@@ -4297,8 +5751,11 @@
       <c r="G96" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J96" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>79</v>
       </c>
@@ -4318,8 +5775,14 @@
       <c r="H97" s="1" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J97" t="s">
+        <v>771</v>
+      </c>
+      <c r="K97" s="1" t="s">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>79</v>
       </c>
@@ -4344,8 +5807,17 @@
       <c r="I98" s="1" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J98" t="s">
+        <v>773</v>
+      </c>
+      <c r="K98" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="L98" s="1" t="s">
+        <v>775</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>79</v>
       </c>
@@ -4370,8 +5842,17 @@
       <c r="I99" s="1" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J99" t="s">
+        <v>776</v>
+      </c>
+      <c r="K99" s="1" t="s">
+        <v>777</v>
+      </c>
+      <c r="L99" s="1" t="s">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>79</v>
       </c>
@@ -4391,8 +5872,14 @@
       <c r="H100" s="1" t="s">
         <v>419</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J100" t="s">
+        <v>779</v>
+      </c>
+      <c r="K100" s="1" t="s">
+        <v>780</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>79</v>
       </c>
@@ -4412,8 +5899,14 @@
       <c r="H101" s="1" t="s">
         <v>420</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J101" t="s">
+        <v>781</v>
+      </c>
+      <c r="K101" s="1" t="s">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>79</v>
       </c>
@@ -4433,8 +5926,14 @@
       <c r="H102" s="1" t="s">
         <v>421</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J102" t="s">
+        <v>783</v>
+      </c>
+      <c r="K102" s="1" t="s">
+        <v>784</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>79</v>
       </c>
@@ -4454,8 +5953,14 @@
       <c r="H103" s="1" t="s">
         <v>422</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J103" t="s">
+        <v>785</v>
+      </c>
+      <c r="K103" s="1" t="s">
+        <v>786</v>
+      </c>
+    </row>
+    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>79</v>
       </c>
@@ -4475,8 +5980,14 @@
       <c r="H104" s="1" t="s">
         <v>423</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J104" t="s">
+        <v>787</v>
+      </c>
+      <c r="K104" s="1" t="s">
+        <v>788</v>
+      </c>
+    </row>
+    <row r="105" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>79</v>
       </c>
@@ -4496,8 +6007,14 @@
       <c r="H105" s="1" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J105" t="s">
+        <v>789</v>
+      </c>
+      <c r="K105" s="1" t="s">
+        <v>790</v>
+      </c>
+    </row>
+    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>79</v>
       </c>
@@ -4517,8 +6034,14 @@
       <c r="H106" s="1" t="s">
         <v>425</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J106" t="s">
+        <v>791</v>
+      </c>
+      <c r="K106" s="1" t="s">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="107" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>79</v>
       </c>
@@ -4538,8 +6061,14 @@
       <c r="H107" s="1" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J107" t="s">
+        <v>793</v>
+      </c>
+      <c r="K107" s="1" t="s">
+        <v>794</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>79</v>
       </c>
@@ -4559,8 +6088,14 @@
       <c r="H108" s="1" t="s">
         <v>427</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J108" t="s">
+        <v>795</v>
+      </c>
+      <c r="K108" s="1" t="s">
+        <v>796</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>79</v>
       </c>
@@ -4580,8 +6115,14 @@
       <c r="H109" s="1" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J109" t="s">
+        <v>797</v>
+      </c>
+      <c r="K109" s="1" t="s">
+        <v>798</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>79</v>
       </c>
@@ -4601,8 +6142,14 @@
       <c r="H110" s="1" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J110" t="s">
+        <v>799</v>
+      </c>
+      <c r="K110" s="1" t="s">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B111">
         <v>2</v>
       </c>
@@ -4614,8 +6161,11 @@
       <c r="G111" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J111" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>79</v>
       </c>
@@ -4635,8 +6185,14 @@
       <c r="H112" s="1" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="J112" t="s">
+        <v>802</v>
+      </c>
+      <c r="K112" s="1" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>79</v>
       </c>
@@ -4656,8 +6212,14 @@
       <c r="H113" s="1" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="114" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J113" t="s">
+        <v>804</v>
+      </c>
+      <c r="K113" s="1" t="s">
+        <v>805</v>
+      </c>
+    </row>
+    <row r="114" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>79</v>
       </c>
@@ -4677,8 +6239,14 @@
       <c r="H114" s="1" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="115" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J114" t="s">
+        <v>806</v>
+      </c>
+      <c r="K114" s="1" t="s">
+        <v>807</v>
+      </c>
+    </row>
+    <row r="115" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>79</v>
       </c>
@@ -4698,8 +6266,14 @@
       <c r="H115" s="1" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J115" t="s">
+        <v>808</v>
+      </c>
+      <c r="K115" s="1" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B116">
         <v>1</v>
       </c>
@@ -4711,8 +6285,11 @@
       <c r="G116" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="117" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J116" t="s">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="117" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>79</v>
       </c>
@@ -4732,8 +6309,14 @@
       <c r="H117" s="1" t="s">
         <v>436</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J117" t="s">
+        <v>811</v>
+      </c>
+      <c r="K117" s="1" t="s">
+        <v>812</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>79</v>
       </c>
@@ -4758,8 +6341,17 @@
       <c r="I118" s="1" t="s">
         <v>438</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J118" t="s">
+        <v>813</v>
+      </c>
+      <c r="K118" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="L118" s="1" t="s">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>79</v>
       </c>
@@ -4779,8 +6371,14 @@
       <c r="H119" s="1" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="J119" t="s">
+        <v>816</v>
+      </c>
+      <c r="K119" s="1" t="s">
+        <v>817</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>79</v>
       </c>
@@ -4800,8 +6398,14 @@
       <c r="H120" s="1" t="s">
         <v>440</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J120" t="s">
+        <v>818</v>
+      </c>
+      <c r="K120" s="1" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="121" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>79</v>
       </c>
@@ -4821,8 +6425,14 @@
       <c r="H121" s="1" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="122" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J121" t="s">
+        <v>820</v>
+      </c>
+      <c r="K121" s="1" t="s">
+        <v>821</v>
+      </c>
+    </row>
+    <row r="122" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>79</v>
       </c>
@@ -4842,8 +6452,14 @@
       <c r="H122" s="1" t="s">
         <v>442</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J122" t="s">
+        <v>822</v>
+      </c>
+      <c r="K122" s="1" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>79</v>
       </c>
@@ -4868,8 +6484,17 @@
       <c r="I123" s="1" t="s">
         <v>444</v>
       </c>
-    </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J123" t="s">
+        <v>824</v>
+      </c>
+      <c r="K123" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="L123" s="1" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>79</v>
       </c>
@@ -4889,8 +6514,14 @@
       <c r="H124" s="1" t="s">
         <v>445</v>
       </c>
-    </row>
-    <row r="125" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J124" t="s">
+        <v>827</v>
+      </c>
+      <c r="K124" s="1" t="s">
+        <v>828</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>79</v>
       </c>
@@ -4910,8 +6541,14 @@
       <c r="H125" s="1" t="s">
         <v>446</v>
       </c>
-    </row>
-    <row r="126" spans="1:9" ht="72" x14ac:dyDescent="0.3">
+      <c r="J125" t="s">
+        <v>829</v>
+      </c>
+      <c r="K125" s="1" t="s">
+        <v>830</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>79</v>
       </c>
@@ -4936,8 +6573,17 @@
       <c r="I126" s="1" t="s">
         <v>448</v>
       </c>
-    </row>
-    <row r="127" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="J126" t="s">
+        <v>831</v>
+      </c>
+      <c r="K126" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="L126" s="1" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>79</v>
       </c>
@@ -4957,8 +6603,14 @@
       <c r="H127" s="1" t="s">
         <v>449</v>
       </c>
-    </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="J127" t="s">
+        <v>834</v>
+      </c>
+      <c r="K127" s="1" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B128">
         <v>1</v>
       </c>
@@ -4970,8 +6622,11 @@
       <c r="G128" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="129" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="J128" t="s">
+        <v>836</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>79</v>
       </c>
@@ -4991,8 +6646,14 @@
       <c r="H129" s="1" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J129" t="s">
+        <v>837</v>
+      </c>
+      <c r="K129" s="1" t="s">
+        <v>838</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B130">
         <v>1</v>
       </c>
@@ -5004,8 +6665,11 @@
       <c r="G130" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J130" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B131">
         <v>2</v>
       </c>
@@ -5017,8 +6681,11 @@
       <c r="G131" t="s">
         <v>453</v>
       </c>
-    </row>
-    <row r="132" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="J131" t="s">
+        <v>840</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="B132">
         <v>3</v>
       </c>
@@ -5029,14 +6696,20 @@
         <v>295</v>
       </c>
       <c r="F132" s="1"/>
-      <c r="G132" s="3" t="s">
+      <c r="G132" t="s">
         <v>572</v>
       </c>
       <c r="H132" s="1" t="s">
         <v>454</v>
       </c>
-    </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="J132" t="s">
+        <v>841</v>
+      </c>
+      <c r="K132" s="1" t="s">
+        <v>842</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B133">
         <v>2</v>
       </c>
@@ -5048,8 +6721,12 @@
       <c r="G133" t="s">
         <v>455</v>
       </c>
-    </row>
-    <row r="134" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="J133" t="s">
+        <v>843</v>
+      </c>
+      <c r="L133"/>
+    </row>
+    <row r="134" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B134">
         <v>3</v>
       </c>
@@ -5060,12 +6737,19 @@
         <v>298</v>
       </c>
       <c r="F134" s="1"/>
-      <c r="G134" s="4" t="s">
+      <c r="G134" t="s">
         <v>573</v>
       </c>
       <c r="H134" s="1" t="s">
         <v>456</v>
       </c>
+      <c r="J134" t="s">
+        <v>844</v>
+      </c>
+      <c r="K134" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="L134"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>